<commit_message>
Update Gradient Boosting A3-test.xlsx
</commit_message>
<xml_diff>
--- a/Testing/Gradient Boosting/Gradient Boosting A3-test.xlsx
+++ b/Testing/Gradient Boosting/Gradient Boosting A3-test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\snegan\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\snegan\Documents\GitHub\AI-Build-Carbon-Predictor\Testing\Gradient Boosting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F092B84-90E2-40BD-8094-A318B0D56930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E3CCF3-D708-46A4-A9E6-B170B82F5789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-75" yWindow="480" windowWidth="28950" windowHeight="15195" activeTab="3" xr2:uid="{6116500C-B190-4EBE-B355-08CA68FBD133}"/>
+    <workbookView xWindow="0" yWindow="405" windowWidth="28950" windowHeight="15195" activeTab="3" xr2:uid="{6116500C-B190-4EBE-B355-08CA68FBD133}"/>
   </bookViews>
   <sheets>
     <sheet name=" Gradient Boositng A3" sheetId="1" r:id="rId1"/>
@@ -782,12 +782,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -818,6 +812,12 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -4396,7 +4396,7 @@
         <xdr:cNvPr id="2" name="Straight Arrow Connector 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7AC7BFC-8988-4B6C-A5E1-E717F19800F9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4449,7 +4449,7 @@
         <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{421415CE-3A24-44EA-BBC6-DB54D6D737C9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4502,7 +4502,7 @@
         <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84759921-2D3C-4D05-8C24-61D6FDECB585}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4555,7 +4555,7 @@
         <xdr:cNvPr id="8" name="Straight Arrow Connector 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1BF54669-3CB5-4C3A-8316-632468D871B2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4608,7 +4608,7 @@
         <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99A30BB0-1BE1-4F58-803D-0FECE1D4EEBF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4661,7 +4661,7 @@
         <xdr:cNvPr id="10" name="Straight Arrow Connector 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{825AD946-78A8-4C61-8376-A6A573B3C691}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4716,7 +4716,7 @@
             <xdr:cNvPr id="11" name="Group 10">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD6F2D69-8B67-42CB-8FF7-9765D2C90F79}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000B000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4738,7 +4738,7 @@
                     <a14:compatExt spid="_x0000_s4097"/>
                   </a:ext>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000010C0000}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000001100000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -4787,7 +4787,7 @@
                     <a14:compatExt spid="_x0000_s4098"/>
                   </a:ext>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000020C0000}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002100000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -4836,7 +4836,7 @@
                     <a14:compatExt spid="_x0000_s4099"/>
                   </a:ext>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000030C0000}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003100000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -4901,7 +4901,7 @@
         <xdr:cNvPr id="12" name="Straight Arrow Connector 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE958624-B4BE-4AB6-B0CA-212F08D29A38}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4954,7 +4954,7 @@
         <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8481CA22-CD7D-494A-AA0E-E7DFFFC5C975}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5007,7 +5007,7 @@
         <xdr:cNvPr id="15" name="Straight Arrow Connector 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3B04581-8F9A-4F2F-8C4B-708C1E990695}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5060,7 +5060,7 @@
         <xdr:cNvPr id="16" name="Straight Arrow Connector 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2A57F2E-8CF3-4A4B-8F18-5133AE29A2C7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000010000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5113,7 +5113,7 @@
         <xdr:cNvPr id="17" name="Straight Arrow Connector 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77D407EA-E929-4C21-8460-AEA86569AB0B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5166,7 +5166,7 @@
         <xdr:cNvPr id="18" name="Straight Arrow Connector 17">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC902BF2-96E7-4D36-8BB2-29C79A6EF4CF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000012000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5228,10 +5228,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="100" xr:uid="{CDABE341-48E2-4EBD-80F7-04BA311A2BD2}" name="Table465859101" displayName="Table465859101" ref="V21:Y27" totalsRowShown="0">
   <autoFilter ref="V21:Y27" xr:uid="{CDABE341-48E2-4EBD-80F7-04BA311A2BD2}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{749B0038-2767-47B7-9728-CE885A6E884F}" name="Learning Rate" dataDxfId="30"/>
-    <tableColumn id="2" xr3:uid="{12DC80AE-8A30-4A52-9948-70254858D46D}" name="Accuracy (%)" dataDxfId="29"/>
+    <tableColumn id="1" xr3:uid="{749B0038-2767-47B7-9728-CE885A6E884F}" name="Learning Rate" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{12DC80AE-8A30-4A52-9948-70254858D46D}" name="Accuracy (%)" dataDxfId="27"/>
     <tableColumn id="3" xr3:uid="{863B55AB-F189-4BD3-BF02-53BA01557603}" name="Time taken (t) / s"/>
-    <tableColumn id="5" xr3:uid="{40B2A0F5-1F51-48E8-874D-1BF6AB964944}" name="Performance (1/t)" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{40B2A0F5-1F51-48E8-874D-1BF6AB964944}" name="Performance (1/t)" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5241,10 +5241,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="101" xr:uid="{7EBB5BCA-94D8-492E-943F-BB9645CE9286}" name="Table46585927102" displayName="Table46585927102" ref="V30:Y36" totalsRowShown="0">
   <autoFilter ref="V30:Y36" xr:uid="{7EBB5BCA-94D8-492E-943F-BB9645CE9286}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{1EBACAC7-0013-49FD-9944-543AB5300858}" name="Learning Rate" dataDxfId="27"/>
+    <tableColumn id="1" xr3:uid="{1EBACAC7-0013-49FD-9944-543AB5300858}" name="Learning Rate" dataDxfId="25"/>
     <tableColumn id="2" xr3:uid="{343C54FA-9323-4657-975E-F4FABDD0DB20}" name="Accuracy (%)"/>
     <tableColumn id="3" xr3:uid="{FD373872-F4A9-4BBC-91FA-80AEB4882B8F}" name="Time taken (t) / s"/>
-    <tableColumn id="5" xr3:uid="{8C7F7FE5-8B4B-433C-ADAE-E7CF64E60CC8}" name="Performance (1/t)" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{8C7F7FE5-8B4B-433C-ADAE-E7CF64E60CC8}" name="Performance (1/t)" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6113,10 +6113,10 @@
 </file>
 
 <file path=xl/tables/table67.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="67" xr:uid="{5465D290-D620-4A15-A2F8-52B3A46FFB29}" name="Table614305256" displayName="Table614305256" ref="G18:G24" totalsRowShown="0" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="67" xr:uid="{5465D290-D620-4A15-A2F8-52B3A46FFB29}" name="Table614305256" displayName="Table614305256" ref="G18:G24" totalsRowShown="0" dataDxfId="64">
   <autoFilter ref="G18:G24" xr:uid="{5465D290-D620-4A15-A2F8-52B3A46FFB29}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{218687D0-4142-4F8D-8DB4-85D681EF8A97}" name="Test case 2.0" dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{218687D0-4142-4F8D-8DB4-85D681EF8A97}" name="Test case 2.0" dataDxfId="63"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6133,10 +6133,10 @@
 </file>
 
 <file path=xl/tables/table69.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="69" xr:uid="{0EAAF75D-2BD3-487F-B377-78E8F46EE047}" name="Table614305258" displayName="Table614305258" ref="G26:G32" totalsRowShown="0" dataDxfId="64">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="69" xr:uid="{0EAAF75D-2BD3-487F-B377-78E8F46EE047}" name="Table614305258" displayName="Table614305258" ref="G26:G32" totalsRowShown="0" dataDxfId="62">
   <autoFilter ref="G26:G32" xr:uid="{0EAAF75D-2BD3-487F-B377-78E8F46EE047}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{47220119-16BF-471A-8532-966A2CBCB501}" name="Test case 2.0" dataDxfId="63"/>
+    <tableColumn id="1" xr3:uid="{47220119-16BF-471A-8532-966A2CBCB501}" name="Test case 2.0" dataDxfId="61"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6163,10 +6163,10 @@
 </file>
 
 <file path=xl/tables/table71.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="71" xr:uid="{850DCFE0-17CE-4D6D-8E50-F0CD3064CCD2}" name="Table614305260" displayName="Table614305260" ref="G34:G40" totalsRowShown="0" dataDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="71" xr:uid="{850DCFE0-17CE-4D6D-8E50-F0CD3064CCD2}" name="Table614305260" displayName="Table614305260" ref="G34:G40" totalsRowShown="0" dataDxfId="60">
   <autoFilter ref="G34:G40" xr:uid="{850DCFE0-17CE-4D6D-8E50-F0CD3064CCD2}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{A50AD645-C3A3-4DC5-9D95-6C81764D08CD}" name="Test case 2.0" dataDxfId="61"/>
+    <tableColumn id="1" xr3:uid="{A50AD645-C3A3-4DC5-9D95-6C81764D08CD}" name="Test case 2.0" dataDxfId="59"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6183,20 +6183,20 @@
 </file>
 
 <file path=xl/tables/table73.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="73" xr:uid="{F01AE6E8-80F4-47C5-9EBB-093F892E91AC}" name="Table614305262" displayName="Table614305262" ref="G42:G48" totalsRowShown="0" dataDxfId="60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="73" xr:uid="{F01AE6E8-80F4-47C5-9EBB-093F892E91AC}" name="Table614305262" displayName="Table614305262" ref="G42:G48" totalsRowShown="0" dataDxfId="58">
   <autoFilter ref="G42:G48" xr:uid="{F01AE6E8-80F4-47C5-9EBB-093F892E91AC}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{25F75ABF-75AE-4C4A-8475-EFABB3E35BEB}" name="Test case 2.0" dataDxfId="59"/>
+    <tableColumn id="1" xr3:uid="{25F75ABF-75AE-4C4A-8475-EFABB3E35BEB}" name="Test case 2.0" dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table74.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="74" xr:uid="{B68821F9-DDB9-4D95-B1B0-FA210E7BE89D}" name="Table6141675" displayName="Table6141675" ref="L2:L8" totalsRowShown="0" dataDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="74" xr:uid="{B68821F9-DDB9-4D95-B1B0-FA210E7BE89D}" name="Table6141675" displayName="Table6141675" ref="L2:L8" totalsRowShown="0" dataDxfId="56">
   <autoFilter ref="L2:L8" xr:uid="{B68821F9-DDB9-4D95-B1B0-FA210E7BE89D}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{2F969AE0-9DE6-485C-80D0-40EEB96177CF}" name="Test case 3.0" dataDxfId="57"/>
+    <tableColumn id="1" xr3:uid="{2F969AE0-9DE6-485C-80D0-40EEB96177CF}" name="Test case 3.0" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6213,10 +6213,10 @@
 </file>
 
 <file path=xl/tables/table76.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="76" xr:uid="{F72EBC0E-55E3-44C5-9A52-7D09BC99FF4C}" name="Table614167577" displayName="Table614167577" ref="L10:L16" totalsRowShown="0" dataDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="76" xr:uid="{F72EBC0E-55E3-44C5-9A52-7D09BC99FF4C}" name="Table614167577" displayName="Table614167577" ref="L10:L16" totalsRowShown="0" dataDxfId="54">
   <autoFilter ref="L10:L16" xr:uid="{F72EBC0E-55E3-44C5-9A52-7D09BC99FF4C}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{30466062-40EE-4F8A-B39D-792FEA647E26}" name="Test case 3.0" dataDxfId="55"/>
+    <tableColumn id="1" xr3:uid="{30466062-40EE-4F8A-B39D-792FEA647E26}" name="Test case 3.0" dataDxfId="53"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6233,10 +6233,10 @@
 </file>
 
 <file path=xl/tables/table78.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="78" xr:uid="{3C14E2D7-4900-4F09-9366-C56F123F20E6}" name="Table614167579" displayName="Table614167579" ref="L18:L24" totalsRowShown="0" dataDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="78" xr:uid="{3C14E2D7-4900-4F09-9366-C56F123F20E6}" name="Table614167579" displayName="Table614167579" ref="L18:L24" totalsRowShown="0" dataDxfId="52">
   <autoFilter ref="L18:L24" xr:uid="{3C14E2D7-4900-4F09-9366-C56F123F20E6}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{BDA91CE6-D252-4E08-8227-F3252E4E0496}" name="Test case 3.0" dataDxfId="53"/>
+    <tableColumn id="1" xr3:uid="{BDA91CE6-D252-4E08-8227-F3252E4E0496}" name="Test case 3.0" dataDxfId="51"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6263,10 +6263,10 @@
 </file>
 
 <file path=xl/tables/table80.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="80" xr:uid="{5B02E13E-1B0A-47EA-A534-CFA67829C450}" name="Table614167581" displayName="Table614167581" ref="L26:L32" totalsRowShown="0" dataDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="80" xr:uid="{5B02E13E-1B0A-47EA-A534-CFA67829C450}" name="Table614167581" displayName="Table614167581" ref="L26:L32" totalsRowShown="0" dataDxfId="50">
   <autoFilter ref="L26:L32" xr:uid="{5B02E13E-1B0A-47EA-A534-CFA67829C450}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{59862783-540E-4E51-BE80-B28EB585D709}" name="Test case 3.0" dataDxfId="51"/>
+    <tableColumn id="1" xr3:uid="{59862783-540E-4E51-BE80-B28EB585D709}" name="Test case 3.0" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6283,10 +6283,10 @@
 </file>
 
 <file path=xl/tables/table82.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="82" xr:uid="{45207D75-3E85-469B-BA01-A38D85540773}" name="Table614167583" displayName="Table614167583" ref="L34:L40" totalsRowShown="0" dataDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="82" xr:uid="{45207D75-3E85-469B-BA01-A38D85540773}" name="Table614167583" displayName="Table614167583" ref="L34:L40" totalsRowShown="0" dataDxfId="48">
   <autoFilter ref="L34:L40" xr:uid="{45207D75-3E85-469B-BA01-A38D85540773}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{0159D84D-3406-4095-BEDA-98C381B53FC7}" name="Test case 3.0" dataDxfId="49"/>
+    <tableColumn id="1" xr3:uid="{0159D84D-3406-4095-BEDA-98C381B53FC7}" name="Test case 3.0" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6303,10 +6303,10 @@
 </file>
 
 <file path=xl/tables/table84.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="84" xr:uid="{0516D6A6-D6E8-4191-9778-B480A05DC44F}" name="Table614167585" displayName="Table614167585" ref="L42:L48" totalsRowShown="0" dataDxfId="48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="84" xr:uid="{0516D6A6-D6E8-4191-9778-B480A05DC44F}" name="Table614167585" displayName="Table614167585" ref="L42:L48" totalsRowShown="0" dataDxfId="46">
   <autoFilter ref="L42:L48" xr:uid="{0516D6A6-D6E8-4191-9778-B480A05DC44F}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{2CA0230C-69C8-40D6-BFAD-CA5E926D027A}" name="Test case 3.0" dataDxfId="47"/>
+    <tableColumn id="1" xr3:uid="{2CA0230C-69C8-40D6-BFAD-CA5E926D027A}" name="Test case 3.0" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6323,10 +6323,10 @@
 </file>
 
 <file path=xl/tables/table86.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="86" xr:uid="{E4AADACC-19A1-4C41-A0C9-B65507992DC2}" name="Table61416184387" displayName="Table61416184387" ref="Q2:Q8" totalsRowShown="0" dataDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="86" xr:uid="{E4AADACC-19A1-4C41-A0C9-B65507992DC2}" name="Table61416184387" displayName="Table61416184387" ref="Q2:Q8" totalsRowShown="0" dataDxfId="44">
   <autoFilter ref="Q2:Q8" xr:uid="{E4AADACC-19A1-4C41-A0C9-B65507992DC2}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{51878B36-D34B-46A5-BC1D-13D05933DD3D}" name="Test case 4" dataDxfId="45"/>
+    <tableColumn id="1" xr3:uid="{51878B36-D34B-46A5-BC1D-13D05933DD3D}" name="Test case 4" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6343,10 +6343,10 @@
 </file>
 
 <file path=xl/tables/table88.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="88" xr:uid="{0F37C559-4DC8-4AA5-B444-8B6A3A1B1D5C}" name="Table6141618438789" displayName="Table6141618438789" ref="Q10:Q16" totalsRowShown="0" dataDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="88" xr:uid="{0F37C559-4DC8-4AA5-B444-8B6A3A1B1D5C}" name="Table6141618438789" displayName="Table6141618438789" ref="Q10:Q16" totalsRowShown="0" dataDxfId="42">
   <autoFilter ref="Q10:Q16" xr:uid="{0F37C559-4DC8-4AA5-B444-8B6A3A1B1D5C}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{7EB25CDF-A9A4-4AC6-8F83-1CD7D8D2156B}" name="Test case 4" dataDxfId="43"/>
+    <tableColumn id="1" xr3:uid="{7EB25CDF-A9A4-4AC6-8F83-1CD7D8D2156B}" name="Test case 4" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6373,10 +6373,10 @@
 </file>
 
 <file path=xl/tables/table90.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="90" xr:uid="{34AB535A-5E67-49D2-AA09-D0684DFD05C7}" name="Table6141618438791" displayName="Table6141618438791" ref="Q18:Q24" totalsRowShown="0" dataDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="90" xr:uid="{34AB535A-5E67-49D2-AA09-D0684DFD05C7}" name="Table6141618438791" displayName="Table6141618438791" ref="Q18:Q24" totalsRowShown="0" dataDxfId="40">
   <autoFilter ref="Q18:Q24" xr:uid="{34AB535A-5E67-49D2-AA09-D0684DFD05C7}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{59F81A4D-53AD-4248-8CA3-D956A6E75CF5}" name="Test case 4" dataDxfId="41"/>
+    <tableColumn id="1" xr3:uid="{59F81A4D-53AD-4248-8CA3-D956A6E75CF5}" name="Test case 4" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6393,10 +6393,10 @@
 </file>
 
 <file path=xl/tables/table92.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="92" xr:uid="{C6BD5C68-40B5-465C-8D86-85BADE8AFB80}" name="Table6141618438793" displayName="Table6141618438793" ref="Q26:Q32" totalsRowShown="0" dataDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="92" xr:uid="{C6BD5C68-40B5-465C-8D86-85BADE8AFB80}" name="Table6141618438793" displayName="Table6141618438793" ref="Q26:Q32" totalsRowShown="0" dataDxfId="38">
   <autoFilter ref="Q26:Q32" xr:uid="{C6BD5C68-40B5-465C-8D86-85BADE8AFB80}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{36A8F31A-3EC4-401D-99EB-0326CB3F5734}" name="Test case 4" dataDxfId="39"/>
+    <tableColumn id="1" xr3:uid="{36A8F31A-3EC4-401D-99EB-0326CB3F5734}" name="Test case 4" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6413,10 +6413,10 @@
 </file>
 
 <file path=xl/tables/table94.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="94" xr:uid="{C6BB2579-D18F-4CD2-BA2B-D640FDF4C2CE}" name="Table6141618438795" displayName="Table6141618438795" ref="Q34:Q40" totalsRowShown="0" dataDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="94" xr:uid="{C6BB2579-D18F-4CD2-BA2B-D640FDF4C2CE}" name="Table6141618438795" displayName="Table6141618438795" ref="Q34:Q40" totalsRowShown="0" dataDxfId="36">
   <autoFilter ref="Q34:Q40" xr:uid="{C6BB2579-D18F-4CD2-BA2B-D640FDF4C2CE}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{3EE10851-2B2B-4C3A-91CF-794EC920C47C}" name="Test case 4" dataDxfId="37"/>
+    <tableColumn id="1" xr3:uid="{3EE10851-2B2B-4C3A-91CF-794EC920C47C}" name="Test case 4" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6433,10 +6433,10 @@
 </file>
 
 <file path=xl/tables/table96.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="96" xr:uid="{2C769679-EEFA-413B-842B-ACEC689CE1FF}" name="Table6141618438797" displayName="Table6141618438797" ref="Q42:Q48" totalsRowShown="0" dataDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="96" xr:uid="{2C769679-EEFA-413B-842B-ACEC689CE1FF}" name="Table6141618438797" displayName="Table6141618438797" ref="Q42:Q48" totalsRowShown="0" dataDxfId="34">
   <autoFilter ref="Q42:Q48" xr:uid="{2C769679-EEFA-413B-842B-ACEC689CE1FF}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{97225219-AECF-4BD4-9F88-52F1FECCF08A}" name="Test case 4" dataDxfId="35"/>
+    <tableColumn id="1" xr3:uid="{97225219-AECF-4BD4-9F88-52F1FECCF08A}" name="Test case 4" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6456,10 +6456,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="98" xr:uid="{33A965EF-AE11-45FD-BB33-5DE8B592484E}" name="Table4699" displayName="Table4699" ref="V3:Y9" totalsRowShown="0">
   <autoFilter ref="V3:Y9" xr:uid="{33A965EF-AE11-45FD-BB33-5DE8B592484E}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{9836BA3F-BAE2-43DA-BCC9-ACE8977F2142}" name="Learning Rate" dataDxfId="34"/>
+    <tableColumn id="1" xr3:uid="{9836BA3F-BAE2-43DA-BCC9-ACE8977F2142}" name="Learning Rate" dataDxfId="32"/>
     <tableColumn id="2" xr3:uid="{759BD8BE-821C-4E96-9262-5B309F718400}" name="Accuracy (%)"/>
     <tableColumn id="3" xr3:uid="{0241B22C-D974-4588-9ACA-E54784E832F3}" name="Time taken (t) / s"/>
-    <tableColumn id="5" xr3:uid="{CB268E54-D66B-4912-A083-16A43DA0BE98}" name="Performance (1/t)" dataDxfId="33"/>
+    <tableColumn id="5" xr3:uid="{CB268E54-D66B-4912-A083-16A43DA0BE98}" name="Performance (1/t)" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6469,10 +6469,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="99" xr:uid="{2A7C3BFF-2D82-4709-95CA-239C04818150}" name="Table4658100" displayName="Table4658100" ref="V12:Y18" totalsRowShown="0">
   <autoFilter ref="V12:Y18" xr:uid="{2A7C3BFF-2D82-4709-95CA-239C04818150}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{7946E05E-550A-4BCD-991F-29B4A517BADD}" name="Learning Rate" dataDxfId="32"/>
+    <tableColumn id="1" xr3:uid="{7946E05E-550A-4BCD-991F-29B4A517BADD}" name="Learning Rate" dataDxfId="30"/>
     <tableColumn id="2" xr3:uid="{F09AEF54-45C8-4E99-B57D-D93E94297FAB}" name="Accuracy (%)"/>
     <tableColumn id="3" xr3:uid="{C279033A-2B9B-4ED8-9EC2-D4DB9C91A394}" name="Time taken (t) / s"/>
-    <tableColumn id="5" xr3:uid="{F3637DE1-7768-4656-9AB0-DBFDD2AEEEF0}" name="Performance (1/t)" dataDxfId="31"/>
+    <tableColumn id="5" xr3:uid="{F3637DE1-7768-4656-9AB0-DBFDD2AEEEF0}" name="Performance (1/t)" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -10735,8 +10735,8 @@
   </sheetPr>
   <dimension ref="B2:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Completed Gradient Boosting Test for A3
</commit_message>
<xml_diff>
--- a/Testing/Gradient Boosting/Gradient Boosting A3-test.xlsx
+++ b/Testing/Gradient Boosting/Gradient Boosting A3-test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\snegan\Documents\GitHub\AI-Build-Carbon-Predictor\Testing\Gradient Boosting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\snegan\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E3CCF3-D708-46A4-A9E6-B170B82F5789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB3817B3-CBAB-4AE4-BDEF-924285822863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="405" windowWidth="28950" windowHeight="15195" activeTab="3" xr2:uid="{6116500C-B190-4EBE-B355-08CA68FBD133}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{6116500C-B190-4EBE-B355-08CA68FBD133}"/>
   </bookViews>
   <sheets>
     <sheet name=" Gradient Boositng A3" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="73">
   <si>
     <t>Gradient Boosting -Test Cases</t>
   </si>
@@ -477,6 +477,89 @@
   <si>
     <t>Limit Depth : 6</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Limit Depth : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>6</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Limit Depth : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Limit Depth : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Limit Depth : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Limit Depth : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <t>Limit Depth</t>
+  </si>
 </sst>
 </file>
 
@@ -674,7 +757,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -702,13 +785,72 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="135">
+  <dxfs count="153">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -4700,16 +4842,16 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor>
         <xdr:from>
-          <xdr:col>18</xdr:col>
-          <xdr:colOff>161925</xdr:colOff>
-          <xdr:row>1</xdr:row>
-          <xdr:rowOff>95250</xdr:rowOff>
+          <xdr:col>20</xdr:col>
+          <xdr:colOff>183573</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>30307</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>20</xdr:col>
-          <xdr:colOff>400050</xdr:colOff>
-          <xdr:row>8</xdr:row>
-          <xdr:rowOff>57150</xdr:rowOff>
+          <xdr:col>22</xdr:col>
+          <xdr:colOff>425162</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>58882</xdr:rowOff>
         </xdr:to>
         <xdr:grpSp>
           <xdr:nvGrpSpPr>
@@ -4724,8 +4866,8 @@
           </xdr:nvGrpSpPr>
           <xdr:grpSpPr>
             <a:xfrm>
-              <a:off x="12763500" y="285750"/>
-              <a:ext cx="1457325" cy="1295400"/>
+              <a:off x="17347623" y="477982"/>
+              <a:ext cx="1460789" cy="1381125"/>
               <a:chOff x="5105400" y="504825"/>
               <a:chExt cx="1457325" cy="1143000"/>
             </a:xfrm>
@@ -5201,6 +5343,324 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>175846</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>7327</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>176698</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98F7139B-5E13-4381-8334-1B66A7D960DA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="14525625" y="814021"/>
+          <a:ext cx="616927" cy="852"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>175846</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>7327</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>176698</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0E6C3BD-AED6-4FC3-A2B3-AD4018992205}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10058400" y="747346"/>
+          <a:ext cx="616927" cy="852"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>175846</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>7327</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>176698</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D777B2A3-B0C8-4965-A5CC-0875E16C9564}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10058400" y="747346"/>
+          <a:ext cx="616927" cy="852"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>175846</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>7327</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>176698</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Straight Arrow Connector 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80CCD1FC-6572-4C53-A073-CC7FB8879264}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10058400" y="3795346"/>
+          <a:ext cx="616927" cy="852"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>175846</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>7327</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>176698</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Straight Arrow Connector 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{117B3A2D-E69B-4AAC-A1A4-446C9550F1C0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10058400" y="5319346"/>
+          <a:ext cx="616927" cy="852"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>175846</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>7327</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>176698</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Straight Arrow Connector 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{660F7281-1F2B-4BE7-84F9-487164D5B33A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10058400" y="5319346"/>
+          <a:ext cx="616927" cy="852"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5215,10 +5675,10 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{12251120-0DF8-4B22-BB50-B9862A8A9E8D}" name="Table62224" displayName="Table62224" ref="B18:B24" totalsRowShown="0" dataDxfId="125">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{12251120-0DF8-4B22-BB50-B9862A8A9E8D}" name="Table62224" displayName="Table62224" ref="B18:B24" totalsRowShown="0" dataDxfId="143">
   <autoFilter ref="B18:B24" xr:uid="{12251120-0DF8-4B22-BB50-B9862A8A9E8D}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{ABBA8AF8-72F0-41A5-918D-E79177B0A42A}" name="Test case 1.2" dataDxfId="124"/>
+    <tableColumn id="1" xr3:uid="{ABBA8AF8-72F0-41A5-918D-E79177B0A42A}" name="Test case 1.2" dataDxfId="142"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5228,10 +5688,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="100" xr:uid="{CDABE341-48E2-4EBD-80F7-04BA311A2BD2}" name="Table465859101" displayName="Table465859101" ref="V21:Y27" totalsRowShown="0">
   <autoFilter ref="V21:Y27" xr:uid="{CDABE341-48E2-4EBD-80F7-04BA311A2BD2}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{749B0038-2767-47B7-9728-CE885A6E884F}" name="Learning Rate" dataDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{12DC80AE-8A30-4A52-9948-70254858D46D}" name="Accuracy (%)" dataDxfId="27"/>
+    <tableColumn id="1" xr3:uid="{749B0038-2767-47B7-9728-CE885A6E884F}" name="Learning Rate" dataDxfId="46"/>
+    <tableColumn id="2" xr3:uid="{12DC80AE-8A30-4A52-9948-70254858D46D}" name="Accuracy (%)" dataDxfId="45"/>
     <tableColumn id="3" xr3:uid="{863B55AB-F189-4BD3-BF02-53BA01557603}" name="Time taken (t) / s"/>
-    <tableColumn id="5" xr3:uid="{40B2A0F5-1F51-48E8-874D-1BF6AB964944}" name="Performance (1/t)" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{40B2A0F5-1F51-48E8-874D-1BF6AB964944}" name="Performance (1/t)" dataDxfId="44"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5241,20 +5701,20 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="101" xr:uid="{7EBB5BCA-94D8-492E-943F-BB9645CE9286}" name="Table46585927102" displayName="Table46585927102" ref="V30:Y36" totalsRowShown="0">
   <autoFilter ref="V30:Y36" xr:uid="{7EBB5BCA-94D8-492E-943F-BB9645CE9286}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{1EBACAC7-0013-49FD-9944-543AB5300858}" name="Learning Rate" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{1EBACAC7-0013-49FD-9944-543AB5300858}" name="Learning Rate" dataDxfId="43"/>
     <tableColumn id="2" xr3:uid="{343C54FA-9323-4657-975E-F4FABDD0DB20}" name="Accuracy (%)"/>
     <tableColumn id="3" xr3:uid="{FD373872-F4A9-4BBC-91FA-80AEB4882B8F}" name="Time taken (t) / s"/>
-    <tableColumn id="5" xr3:uid="{8C7F7FE5-8B4B-433C-ADAE-E7CF64E60CC8}" name="Performance (1/t)" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{8C7F7FE5-8B4B-433C-ADAE-E7CF64E60CC8}" name="Performance (1/t)" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table102.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="102" xr:uid="{9BA039EE-CBD9-46B4-BB31-982822EF9567}" name="Table6226567103" displayName="Table6226567103" ref="B2:B8" totalsRowShown="0" dataDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="102" xr:uid="{9BA039EE-CBD9-46B4-BB31-982822EF9567}" name="Table6226567103" displayName="Table6226567103" ref="B2:B8" totalsRowShown="0" dataDxfId="41">
   <autoFilter ref="B2:B8" xr:uid="{9BA039EE-CBD9-46B4-BB31-982822EF9567}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{68E6C729-D6F4-4C9D-BD38-7213A17EDC58}" name="Test case 1.0" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{68E6C729-D6F4-4C9D-BD38-7213A17EDC58}" name="Test case 1.0" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5271,10 +5731,10 @@
 </file>
 
 <file path=xl/tables/table104.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="104" xr:uid="{609934ED-C17F-4B57-A771-D07D334C6A87}" name="Table6226567103105" displayName="Table6226567103105" ref="B10:B16" totalsRowShown="0" dataDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="104" xr:uid="{609934ED-C17F-4B57-A771-D07D334C6A87}" name="Table6226567103105" displayName="Table6226567103105" ref="B10:B16" totalsRowShown="0" dataDxfId="39">
   <autoFilter ref="B10:B16" xr:uid="{609934ED-C17F-4B57-A771-D07D334C6A87}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{B262A5BF-07B5-4872-8BB1-4299CC330833}" name="Test case 1.0" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{B262A5BF-07B5-4872-8BB1-4299CC330833}" name="Test case 1.0" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5291,10 +5751,10 @@
 </file>
 
 <file path=xl/tables/table106.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="106" xr:uid="{F36C72A3-E8F2-4A90-8EA1-3899CE6E92AC}" name="Table6226567103107" displayName="Table6226567103107" ref="B18:B24" totalsRowShown="0" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="106" xr:uid="{F36C72A3-E8F2-4A90-8EA1-3899CE6E92AC}" name="Table6226567103107" displayName="Table6226567103107" ref="B18:B24" totalsRowShown="0" dataDxfId="37">
   <autoFilter ref="B18:B24" xr:uid="{F36C72A3-E8F2-4A90-8EA1-3899CE6E92AC}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{4F43328F-1BFE-4B5B-A24F-934A79A13DB0}" name="Test case 1.0" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{4F43328F-1BFE-4B5B-A24F-934A79A13DB0}" name="Test case 1.0" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5311,10 +5771,10 @@
 </file>
 
 <file path=xl/tables/table108.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="108" xr:uid="{8D79F858-D9FA-495E-B7E2-D41AC26F87EF}" name="Table6226567103109" displayName="Table6226567103109" ref="B26:B32" totalsRowShown="0" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="108" xr:uid="{8D79F858-D9FA-495E-B7E2-D41AC26F87EF}" name="Table6226567103109" displayName="Table6226567103109" ref="B26:B32" totalsRowShown="0" dataDxfId="35">
   <autoFilter ref="B26:B32" xr:uid="{8D79F858-D9FA-495E-B7E2-D41AC26F87EF}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{AFEEEB04-1011-470C-84DF-5DFAA9B9511E}" name="Test case 1.0" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{AFEEEB04-1011-470C-84DF-5DFAA9B9511E}" name="Test case 1.0" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5341,10 +5801,10 @@
 </file>
 
 <file path=xl/tables/table110.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="110" xr:uid="{FDE3A9D9-4732-4BAE-B3C3-716CDA104EE2}" name="Table6226567103111" displayName="Table6226567103111" ref="B34:B40" totalsRowShown="0" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="110" xr:uid="{FDE3A9D9-4732-4BAE-B3C3-716CDA104EE2}" name="Table6226567103111" displayName="Table6226567103111" ref="B34:B40" totalsRowShown="0" dataDxfId="33">
   <autoFilter ref="B34:B40" xr:uid="{FDE3A9D9-4732-4BAE-B3C3-716CDA104EE2}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{6BF6E735-5A81-4D61-BDDF-6764A9FED46D}" name="Test case 1.0" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{6BF6E735-5A81-4D61-BDDF-6764A9FED46D}" name="Test case 1.0" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5361,10 +5821,10 @@
 </file>
 
 <file path=xl/tables/table112.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="112" xr:uid="{1E324EA0-0DA5-49BE-95DB-E177900F5748}" name="Table6226567103113" displayName="Table6226567103113" ref="B42:B48" totalsRowShown="0" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="112" xr:uid="{1E324EA0-0DA5-49BE-95DB-E177900F5748}" name="Table6226567103113" displayName="Table6226567103113" ref="B42:B48" totalsRowShown="0" dataDxfId="31">
   <autoFilter ref="B42:B48" xr:uid="{1E324EA0-0DA5-49BE-95DB-E177900F5748}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{C56EF5C4-FFE0-48BC-B6F8-BD31F4E4117A}" name="Test case 1.0" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{C56EF5C4-FFE0-48BC-B6F8-BD31F4E4117A}" name="Test case 1.0" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5391,10 +5851,10 @@
 </file>
 
 <file path=xl/tables/table115.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="115" xr:uid="{3093D378-765C-4E13-A37B-A0400626E62F}" name="Table614305256116" displayName="Table614305256116" ref="G2:G8" totalsRowShown="0" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="115" xr:uid="{3093D378-765C-4E13-A37B-A0400626E62F}" name="Table614305256116" displayName="Table614305256116" ref="G2:G8" totalsRowShown="0" dataDxfId="29">
   <autoFilter ref="G2:G8" xr:uid="{3093D378-765C-4E13-A37B-A0400626E62F}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{3B336B95-FBEF-4001-84BF-B099BF0F1C32}" name="Test case 2.0" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{3B336B95-FBEF-4001-84BF-B099BF0F1C32}" name="Test case 2.0" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5411,10 +5871,10 @@
 </file>
 
 <file path=xl/tables/table117.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="117" xr:uid="{5F8A4DB2-C8CE-4DEF-8515-E5206F433390}" name="Table614305256116118" displayName="Table614305256116118" ref="G10:G16" totalsRowShown="0" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="117" xr:uid="{5F8A4DB2-C8CE-4DEF-8515-E5206F433390}" name="Table614305256116118" displayName="Table614305256116118" ref="G10:G16" totalsRowShown="0" dataDxfId="27">
   <autoFilter ref="G10:G16" xr:uid="{5F8A4DB2-C8CE-4DEF-8515-E5206F433390}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{D953F323-92B7-4F49-9C60-CB5F875084FE}" name="Test case 2.0" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{D953F323-92B7-4F49-9C60-CB5F875084FE}" name="Test case 2.0" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5431,46 +5891,36 @@
 </file>
 
 <file path=xl/tables/table119.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="121" xr:uid="{F6697C10-DB4A-4362-8BFE-AD43D85814E7}" name="Table614305256116122" displayName="Table614305256116122" ref="G18:G24" totalsRowShown="0" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="121" xr:uid="{F6697C10-DB4A-4362-8BFE-AD43D85814E7}" name="Table614305256116122" displayName="Table614305256116122" ref="G18:G24" totalsRowShown="0" dataDxfId="25">
   <autoFilter ref="G18:G24" xr:uid="{F6697C10-DB4A-4362-8BFE-AD43D85814E7}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{5B6592BC-3043-488F-BC9F-019DAD203888}" name="Test case 2.0" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{5B6592BC-3043-488F-BC9F-019DAD203888}" name="Test case 2.0" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{3996F55D-63F6-4539-92B4-FF151C3F0759}" name="Table6222426" displayName="Table6222426" ref="B26:B32" totalsRowShown="0" dataDxfId="123">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{3996F55D-63F6-4539-92B4-FF151C3F0759}" name="Table6222426" displayName="Table6222426" ref="B26:B32" totalsRowShown="0" dataDxfId="141">
   <autoFilter ref="B26:B32" xr:uid="{3996F55D-63F6-4539-92B4-FF151C3F0759}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{DF29860F-D319-4EEE-83F9-9BAB4BB72CB8}" name="Test case 1.3" dataDxfId="122"/>
+    <tableColumn id="1" xr3:uid="{DF29860F-D319-4EEE-83F9-9BAB4BB72CB8}" name="Test case 1.3" dataDxfId="140"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table120.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="122" xr:uid="{C931F6F6-3A64-4D94-B1A0-925C175C1A07}" name="Table1215315155115123" displayName="Table1215315155115123" ref="I26:I32" totalsRowShown="0">
-  <autoFilter ref="I26:I32" xr:uid="{C931F6F6-3A64-4D94-B1A0-925C175C1A07}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{05F44034-45A9-456B-991E-98E52B4178E1}" name="Results "/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table121.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="123" xr:uid="{819D1479-B137-44B1-A342-8CD47A1D8937}" name="Table614305256116124" displayName="Table614305256116124" ref="G26:G32" totalsRowShown="0" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="123" xr:uid="{819D1479-B137-44B1-A342-8CD47A1D8937}" name="Table614305256116124" displayName="Table614305256116124" ref="G26:G32" totalsRowShown="0" dataDxfId="23">
   <autoFilter ref="G26:G32" xr:uid="{819D1479-B137-44B1-A342-8CD47A1D8937}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{6EB4ED72-2106-447E-BF6F-4B246F829BA9}" name="Test case 2.0" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{6EB4ED72-2106-447E-BF6F-4B246F829BA9}" name="Test case 2.0" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table122.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table121.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="124" xr:uid="{BEE268EC-2588-44EE-BBFC-99E7C5D2F9BC}" name="Table1215315155115125" displayName="Table1215315155115125" ref="I34:I40" totalsRowShown="0">
   <autoFilter ref="I34:I40" xr:uid="{BEE268EC-2588-44EE-BBFC-99E7C5D2F9BC}"/>
   <tableColumns count="1">
@@ -5480,17 +5930,17 @@
 </table>
 </file>
 
-<file path=xl/tables/table123.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="125" xr:uid="{4E14B564-9597-4E94-A937-205239BC4490}" name="Table614305256116126" displayName="Table614305256116126" ref="G34:G40" totalsRowShown="0" dataDxfId="3">
+<file path=xl/tables/table122.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="125" xr:uid="{4E14B564-9597-4E94-A937-205239BC4490}" name="Table614305256116126" displayName="Table614305256116126" ref="G34:G40" totalsRowShown="0" dataDxfId="21">
   <autoFilter ref="G34:G40" xr:uid="{4E14B564-9597-4E94-A937-205239BC4490}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{C5D46CFD-4A3A-41C7-BE53-00A78820403B}" name="Test case 2.0" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{C5D46CFD-4A3A-41C7-BE53-00A78820403B}" name="Test case 2.0" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table124.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table123.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="126" xr:uid="{91415F22-4C9A-41AE-A99D-7F76D83EC4F4}" name="Table1215315155115127" displayName="Table1215315155115127" ref="I42:I48" totalsRowShown="0">
   <autoFilter ref="I42:I48" xr:uid="{91415F22-4C9A-41AE-A99D-7F76D83EC4F4}"/>
   <tableColumns count="1">
@@ -5500,11 +5950,61 @@
 </table>
 </file>
 
-<file path=xl/tables/table125.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="127" xr:uid="{7CB47E40-D0A8-4F77-A18C-77BC5CABACFC}" name="Table614305256116128" displayName="Table614305256116128" ref="G42:G48" totalsRowShown="0" dataDxfId="1">
+<file path=xl/tables/table124.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="127" xr:uid="{7CB47E40-D0A8-4F77-A18C-77BC5CABACFC}" name="Table614305256116128" displayName="Table614305256116128" ref="G42:G48" totalsRowShown="0" dataDxfId="19">
   <autoFilter ref="G42:G48" xr:uid="{7CB47E40-D0A8-4F77-A18C-77BC5CABACFC}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{D50BAD2C-DF67-4E86-A0F2-F53CD41E69F2}" name="Test case 2.0" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{D50BAD2C-DF67-4E86-A0F2-F53CD41E69F2}" name="Test case 2.0" dataDxfId="18"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table125.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="118" xr:uid="{8D5C2951-E33A-488C-B6D3-A3AE756862BB}" name="Table61416184387119" displayName="Table61416184387119" ref="L2:L8" totalsRowShown="0" dataDxfId="17">
+  <autoFilter ref="L2:L8" xr:uid="{8D5C2951-E33A-488C-B6D3-A3AE756862BB}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{83287009-206F-42B6-83FF-8F6C7F3324A1}" name="Test case 4" dataDxfId="16"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table126.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="119" xr:uid="{5D0D1825-1B85-4C8B-9B1C-38B282B8CF2C}" name="Table121517194488120" displayName="Table121517194488120" ref="N2:N8" totalsRowShown="0">
+  <autoFilter ref="N2:N8" xr:uid="{5D0D1825-1B85-4C8B-9B1C-38B282B8CF2C}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{C44483A2-0512-4AD5-B2B5-C7788B359E08}" name="Results "/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table127.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="128" xr:uid="{110155AD-2E7A-43E5-8C04-18E156C75E9D}" name="Table61416184387119129" displayName="Table61416184387119129" ref="L10:L16" totalsRowShown="0" dataDxfId="15">
+  <autoFilter ref="L10:L16" xr:uid="{110155AD-2E7A-43E5-8C04-18E156C75E9D}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{983925D7-878F-4998-83A8-A763A7EEA57E}" name="Test case 4" dataDxfId="14"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table128.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="129" xr:uid="{87127AB7-4516-4D4C-80D0-76E661BA4C7A}" name="Table121517194488120130" displayName="Table121517194488120130" ref="N10:N16" totalsRowShown="0">
+  <autoFilter ref="N10:N16" xr:uid="{87127AB7-4516-4D4C-80D0-76E661BA4C7A}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{FFFC2668-AD96-4E87-B492-D900AFA6EAB1}" name="Results "/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table129.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="130" xr:uid="{DE482530-3C41-437B-BA6A-816F2FA367E2}" name="Table61416184387119131" displayName="Table61416184387119131" ref="L18:L24" totalsRowShown="0" dataDxfId="13">
+  <autoFilter ref="L18:L24" xr:uid="{DE482530-3C41-437B-BA6A-816F2FA367E2}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{F71417C3-91E8-44A3-8999-56C932C1A506}" name="Test case 4" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5520,11 +6020,130 @@
 </table>
 </file>
 
+<file path=xl/tables/table130.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="131" xr:uid="{B409A0C6-F709-4DD1-B85D-79EB25369974}" name="Table121517194488120132" displayName="Table121517194488120132" ref="N18:N24" totalsRowShown="0">
+  <autoFilter ref="N18:N24" xr:uid="{B409A0C6-F709-4DD1-B85D-79EB25369974}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{19F8688B-15EC-42DA-B6A4-80201F997C1B}" name="Results "/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table131.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="134" xr:uid="{0673B3A9-993D-441E-8DE0-9E234DCC337B}" name="Table61416184387119131135" displayName="Table61416184387119131135" ref="L26:L32" totalsRowShown="0" dataDxfId="11">
+  <autoFilter ref="L26:L32" xr:uid="{0673B3A9-993D-441E-8DE0-9E234DCC337B}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{09683389-F5AB-408B-A7CB-8EB914314F4D}" name="Test case 4" dataDxfId="10"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table132.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="135" xr:uid="{26A14944-3203-4A87-B732-121A6AB30142}" name="Table121517194488120132136" displayName="Table121517194488120132136" ref="N26:N32" totalsRowShown="0">
+  <autoFilter ref="N26:N32" xr:uid="{26A14944-3203-4A87-B732-121A6AB30142}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{CC0E8FD3-8D82-409A-80AC-CBEEE65B880A}" name="Results "/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table133.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="136" xr:uid="{2B497805-90EA-42D6-B60D-4AC5120DF537}" name="Table61416184387119131135137" displayName="Table61416184387119131135137" ref="L34:L40" totalsRowShown="0" dataDxfId="9">
+  <autoFilter ref="L34:L40" xr:uid="{2B497805-90EA-42D6-B60D-4AC5120DF537}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{6238B4FC-131E-46D6-AE46-67FD89E88607}" name="Test case 4" dataDxfId="8"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table134.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="137" xr:uid="{E7324636-2391-4A83-BAF9-5FC75C010318}" name="Table121517194488120132136138" displayName="Table121517194488120132136138" ref="N34:N40" totalsRowShown="0">
+  <autoFilter ref="N34:N40" xr:uid="{E7324636-2391-4A83-BAF9-5FC75C010318}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{DB279BCF-E439-4C7D-AC82-950F626035E4}" name="Results "/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table135.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="138" xr:uid="{900090D3-9AA8-4A3D-B083-5A357D2AA9BB}" name="Table61416184387119131135139" displayName="Table61416184387119131135139" ref="L42:L48" totalsRowShown="0" dataDxfId="7">
+  <autoFilter ref="L42:L48" xr:uid="{900090D3-9AA8-4A3D-B083-5A357D2AA9BB}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{8288319A-ED7E-422D-BD75-D33DA2402956}" name="Test case 4" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table136.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="139" xr:uid="{9A2B8937-A7B3-4CF6-AC1B-3527F05016DC}" name="Table121517194488120132136140" displayName="Table121517194488120132136140" ref="N42:N48" totalsRowShown="0">
+  <autoFilter ref="N42:N48" xr:uid="{9A2B8937-A7B3-4CF6-AC1B-3527F05016DC}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{7C11E819-71FE-415F-B9AA-1B61AB6E90BE}" name="Results "/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table137.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="140" xr:uid="{D3FC7BEA-4C8E-43D8-BAEC-09167CE0E29E}" name="Table4699141" displayName="Table4699141" ref="Q3:T9" totalsRowShown="0">
+  <autoFilter ref="Q3:T9" xr:uid="{D3FC7BEA-4C8E-43D8-BAEC-09167CE0E29E}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{BD7B119F-09FB-468A-B097-425B2F72D504}" name="Limit Depth" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{A8A93E46-798A-45BA-8A39-F1BE56BAF865}" name="Accuracy (%)"/>
+    <tableColumn id="3" xr3:uid="{B7244C3B-D0B6-4513-A9E3-94550BFB5CC2}" name="Time taken (t) / s"/>
+    <tableColumn id="5" xr3:uid="{B2FD9D41-90B5-4161-A8E9-068A4FBBA72A}" name="Performance (1/t)" dataDxfId="4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table138.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="141" xr:uid="{28C04D4C-2B06-440C-ADEE-29FB443102F1}" name="Table4658100142" displayName="Table4658100142" ref="Q12:T18" totalsRowShown="0">
+  <autoFilter ref="Q12:T18" xr:uid="{28C04D4C-2B06-440C-ADEE-29FB443102F1}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{9DF1E4D4-BBBD-4E8D-B388-7AEF45B7FEA3}" name="Limit Depth" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{3A24D5D1-7B53-4BC4-BADB-D76FDE109070}" name="Accuracy (%)"/>
+    <tableColumn id="3" xr3:uid="{73C55E50-D4AC-41CA-BFB0-42AFAAD9E2D3}" name="Time taken (t) / s"/>
+    <tableColumn id="5" xr3:uid="{8936D0C6-51F8-433D-B47B-B4F7ED14DD83}" name="Performance (1/t)" dataDxfId="3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table139.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="143" xr:uid="{CC8CCA56-8B4A-4341-9123-900F37A66C8A}" name="Table46585927102144" displayName="Table46585927102144" ref="Q21:T27" totalsRowShown="0">
+  <autoFilter ref="Q21:T27" xr:uid="{CC8CCA56-8B4A-4341-9123-900F37A66C8A}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{40D8C5D6-9489-47AA-ACAB-9F7154836790}" name="Limit Depth" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{28F8AF11-0132-41F0-9EF6-CD386129CAAA}" name="Accuracy (%)"/>
+    <tableColumn id="3" xr3:uid="{ADADCCB0-966F-4EAC-A464-0BD236AEBE0C}" name="Time taken (t) / s"/>
+    <tableColumn id="5" xr3:uid="{4DC39A98-D2D0-404A-9DDB-E36413F55DB7}" name="Performance (1/t)" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{DAE3DB0E-16D0-4EB4-BD96-A1E89E8BC7BC}" name="Table622242628" displayName="Table622242628" ref="B34:B40" totalsRowShown="0" dataDxfId="121">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{DAE3DB0E-16D0-4EB4-BD96-A1E89E8BC7BC}" name="Table622242628" displayName="Table622242628" ref="B34:B40" totalsRowShown="0" dataDxfId="139">
   <autoFilter ref="B34:B40" xr:uid="{DAE3DB0E-16D0-4EB4-BD96-A1E89E8BC7BC}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{DE286A69-8F1D-4C8A-82BE-9E158A881EBA}" name="Test case 1.4" dataDxfId="120"/>
+    <tableColumn id="1" xr3:uid="{DE286A69-8F1D-4C8A-82BE-9E158A881EBA}" name="Test case 1.4" dataDxfId="138"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table140.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="122" xr:uid="{C931F6F6-3A64-4D94-B1A0-925C175C1A07}" name="Table1215315155115123" displayName="Table1215315155115123" ref="I26:I32" totalsRowShown="0">
+  <autoFilter ref="I26:I32" xr:uid="{C931F6F6-3A64-4D94-B1A0-925C175C1A07}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{05F44034-45A9-456B-991E-98E52B4178E1}" name="Results "/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5541,10 +6160,10 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{1BCA6073-E4C8-4522-B1E6-967A8B6DED6D}" name="Table614" displayName="Table614" ref="G10:G16" totalsRowShown="0" dataDxfId="119">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{1BCA6073-E4C8-4522-B1E6-967A8B6DED6D}" name="Table614" displayName="Table614" ref="G10:G16" totalsRowShown="0" dataDxfId="137">
   <autoFilter ref="G10:G16" xr:uid="{1BCA6073-E4C8-4522-B1E6-967A8B6DED6D}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{5277FB98-E51D-4D48-8F3A-1FF3AADDD189}" name="Test case 2.1" dataDxfId="118"/>
+    <tableColumn id="1" xr3:uid="{5277FB98-E51D-4D48-8F3A-1FF3AADDD189}" name="Test case 2.1" dataDxfId="136"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5571,20 +6190,20 @@
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{24CE6D52-88EF-4D29-B896-016DFC482570}" name="Table61432" displayName="Table61432" ref="G18:G24" totalsRowShown="0" dataDxfId="117">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{24CE6D52-88EF-4D29-B896-016DFC482570}" name="Table61432" displayName="Table61432" ref="G18:G24" totalsRowShown="0" dataDxfId="135">
   <autoFilter ref="G18:G24" xr:uid="{24CE6D52-88EF-4D29-B896-016DFC482570}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{329CA240-0D45-47F8-8BB6-C75CC6D69270}" name="Test case 2.2" dataDxfId="116"/>
+    <tableColumn id="1" xr3:uid="{329CA240-0D45-47F8-8BB6-C75CC6D69270}" name="Test case 2.2" dataDxfId="134"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AFC44A08-478C-4325-850B-7040C4798DA8}" name="Table2" displayName="Table2" ref="B10:B11" totalsRowShown="0" dataDxfId="134">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AFC44A08-478C-4325-850B-7040C4798DA8}" name="Table2" displayName="Table2" ref="B10:B11" totalsRowShown="0" dataDxfId="152">
   <autoFilter ref="B10:B11" xr:uid="{AFC44A08-478C-4325-850B-7040C4798DA8}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{30A24230-9276-4C3A-9E21-A9DB2ED9BE52}" name="2.Number of Trees" dataDxfId="133"/>
+    <tableColumn id="1" xr3:uid="{30A24230-9276-4C3A-9E21-A9DB2ED9BE52}" name="2.Number of Trees" dataDxfId="151"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5601,10 +6220,10 @@
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{4F6B6FFA-B0B3-4A94-BB0E-03E8C639AAA6}" name="Table61434" displayName="Table61434" ref="G26:G32" totalsRowShown="0" dataDxfId="115">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{4F6B6FFA-B0B3-4A94-BB0E-03E8C639AAA6}" name="Table61434" displayName="Table61434" ref="G26:G32" totalsRowShown="0" dataDxfId="133">
   <autoFilter ref="G26:G32" xr:uid="{4F6B6FFA-B0B3-4A94-BB0E-03E8C639AAA6}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{68EB9801-BEA5-44A6-8885-645DE578BEF1}" name="Test case 2.3" dataDxfId="114"/>
+    <tableColumn id="1" xr3:uid="{68EB9801-BEA5-44A6-8885-645DE578BEF1}" name="Test case 2.3" dataDxfId="132"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5621,20 +6240,20 @@
 </file>
 
 <file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{C3D7949C-F10F-4F90-A4C7-D6CDBFA0638E}" name="Table61430" displayName="Table61430" ref="G2:G8" totalsRowShown="0" dataDxfId="113">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{C3D7949C-F10F-4F90-A4C7-D6CDBFA0638E}" name="Table61430" displayName="Table61430" ref="G2:G8" totalsRowShown="0" dataDxfId="131">
   <autoFilter ref="G2:G8" xr:uid="{C3D7949C-F10F-4F90-A4C7-D6CDBFA0638E}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{D25D01DF-BD5E-4E98-A77B-4417E3284DB5}" name="Test case 2.0" dataDxfId="112"/>
+    <tableColumn id="1" xr3:uid="{D25D01DF-BD5E-4E98-A77B-4417E3284DB5}" name="Test case 2.0" dataDxfId="130"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{8181812F-50EC-46B0-9899-8787EF360FCC}" name="Table6143438" displayName="Table6143438" ref="G34:G40" totalsRowShown="0" dataDxfId="111">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{8181812F-50EC-46B0-9899-8787EF360FCC}" name="Table6143438" displayName="Table6143438" ref="G34:G40" totalsRowShown="0" dataDxfId="129">
   <autoFilter ref="G34:G40" xr:uid="{8181812F-50EC-46B0-9899-8787EF360FCC}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{ABDC1383-2DC6-4746-A71F-443D1857C309}" name="Test case 2.4" dataDxfId="110"/>
+    <tableColumn id="1" xr3:uid="{ABDC1383-2DC6-4746-A71F-443D1857C309}" name="Test case 2.4" dataDxfId="128"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5651,10 +6270,10 @@
 </file>
 
 <file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="36" xr:uid="{304066CF-3C19-42E6-A1BF-948D8C429EE3}" name="Table61416" displayName="Table61416" ref="L2:L8" totalsRowShown="0" dataDxfId="109">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="36" xr:uid="{304066CF-3C19-42E6-A1BF-948D8C429EE3}" name="Table61416" displayName="Table61416" ref="L2:L8" totalsRowShown="0" dataDxfId="127">
   <autoFilter ref="L2:L8" xr:uid="{304066CF-3C19-42E6-A1BF-948D8C429EE3}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{9161523A-0737-4896-A3EA-DEF995A3796C}" name="Test case 3.0" dataDxfId="108"/>
+    <tableColumn id="1" xr3:uid="{9161523A-0737-4896-A3EA-DEF995A3796C}" name="Test case 3.0" dataDxfId="126"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5671,10 +6290,10 @@
 </file>
 
 <file path=xl/tables/table28.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="38" xr:uid="{0912608B-D3A5-4878-8E87-952CEC46A529}" name="Table614168" displayName="Table614168" ref="L10:L16" totalsRowShown="0" dataDxfId="107">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="38" xr:uid="{0912608B-D3A5-4878-8E87-952CEC46A529}" name="Table614168" displayName="Table614168" ref="L10:L16" totalsRowShown="0" dataDxfId="125">
   <autoFilter ref="L10:L16" xr:uid="{0912608B-D3A5-4878-8E87-952CEC46A529}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{EC133DAF-A4F6-4AD1-8F21-1D75494182A4}" name="Test case 3.1" dataDxfId="106"/>
+    <tableColumn id="1" xr3:uid="{EC133DAF-A4F6-4AD1-8F21-1D75494182A4}" name="Test case 3.1" dataDxfId="124"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5691,20 +6310,20 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DFDBF571-5900-4AF1-87EB-98ED6B0C06AD}" name="Table3" displayName="Table3" ref="B13:B15" totalsRowShown="0" headerRowDxfId="132" dataDxfId="131">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DFDBF571-5900-4AF1-87EB-98ED6B0C06AD}" name="Table3" displayName="Table3" ref="B13:B15" totalsRowShown="0" headerRowDxfId="150" dataDxfId="149">
   <autoFilter ref="B13:B15" xr:uid="{DFDBF571-5900-4AF1-87EB-98ED6B0C06AD}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{058796B2-9C99-4CA9-A681-0DF0A1E20243}" name="3.Learning Rate" dataDxfId="130"/>
+    <tableColumn id="1" xr3:uid="{058796B2-9C99-4CA9-A681-0DF0A1E20243}" name="3.Learning Rate" dataDxfId="148"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table30.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="40" xr:uid="{83BCD226-EFDE-4EEE-BB35-5057D0A896FC}" name="Table6141610" displayName="Table6141610" ref="L18:L24" totalsRowShown="0" dataDxfId="105">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="40" xr:uid="{83BCD226-EFDE-4EEE-BB35-5057D0A896FC}" name="Table6141610" displayName="Table6141610" ref="L18:L24" totalsRowShown="0" dataDxfId="123">
   <autoFilter ref="L18:L24" xr:uid="{83BCD226-EFDE-4EEE-BB35-5057D0A896FC}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{1D03115D-59DB-4A50-A65A-9F20F0602DAA}" name="Test case 3" dataDxfId="104"/>
+    <tableColumn id="1" xr3:uid="{1D03115D-59DB-4A50-A65A-9F20F0602DAA}" name="Test case 3" dataDxfId="122"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5721,10 +6340,10 @@
 </file>
 
 <file path=xl/tables/table32.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="42" xr:uid="{CE25E6BE-E364-436A-9DA0-9929B472A71E}" name="Table6141612" displayName="Table6141612" ref="L26:L32" totalsRowShown="0" dataDxfId="103">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="42" xr:uid="{CE25E6BE-E364-436A-9DA0-9929B472A71E}" name="Table6141612" displayName="Table6141612" ref="L26:L32" totalsRowShown="0" dataDxfId="121">
   <autoFilter ref="L26:L32" xr:uid="{CE25E6BE-E364-436A-9DA0-9929B472A71E}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{96242001-8CA1-4EDE-8B99-C4E8DF35F438}" name="Test case 3" dataDxfId="102"/>
+    <tableColumn id="1" xr3:uid="{96242001-8CA1-4EDE-8B99-C4E8DF35F438}" name="Test case 3" dataDxfId="120"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5741,10 +6360,10 @@
 </file>
 
 <file path=xl/tables/table34.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="44" xr:uid="{E43AD37B-4925-458C-B9BD-88F029C9F050}" name="Table6141621" displayName="Table6141621" ref="L34:L40" totalsRowShown="0" dataDxfId="101">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="44" xr:uid="{E43AD37B-4925-458C-B9BD-88F029C9F050}" name="Table6141621" displayName="Table6141621" ref="L34:L40" totalsRowShown="0" dataDxfId="119">
   <autoFilter ref="L34:L40" xr:uid="{E43AD37B-4925-458C-B9BD-88F029C9F050}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{7504A3B4-552E-4686-B691-9AFF1079EC6E}" name="Test case 3" dataDxfId="100"/>
+    <tableColumn id="1" xr3:uid="{7504A3B4-552E-4686-B691-9AFF1079EC6E}" name="Test case 3" dataDxfId="118"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5761,10 +6380,10 @@
 </file>
 
 <file path=xl/tables/table36.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="46" xr:uid="{87A71E5A-F9D8-41DF-A440-F9AE057B748A}" name="Table6141618" displayName="Table6141618" ref="Q2:Q8" totalsRowShown="0" dataDxfId="99">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="46" xr:uid="{87A71E5A-F9D8-41DF-A440-F9AE057B748A}" name="Table6141618" displayName="Table6141618" ref="Q2:Q8" totalsRowShown="0" dataDxfId="117">
   <autoFilter ref="Q2:Q8" xr:uid="{87A71E5A-F9D8-41DF-A440-F9AE057B748A}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{7221A79B-CDA2-400B-9F8B-551D580F16AB}" name="Test case 4" dataDxfId="98"/>
+    <tableColumn id="1" xr3:uid="{7221A79B-CDA2-400B-9F8B-551D580F16AB}" name="Test case 4" dataDxfId="116"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5781,10 +6400,10 @@
 </file>
 
 <file path=xl/tables/table38.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="48" xr:uid="{D24335F9-8187-4CC0-9556-D7011A019966}" name="Table614161837" displayName="Table614161837" ref="Q10:Q16" totalsRowShown="0" dataDxfId="97">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="48" xr:uid="{D24335F9-8187-4CC0-9556-D7011A019966}" name="Table614161837" displayName="Table614161837" ref="Q10:Q16" totalsRowShown="0" dataDxfId="115">
   <autoFilter ref="Q10:Q16" xr:uid="{D24335F9-8187-4CC0-9556-D7011A019966}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{EA26578D-A990-4EA9-9A5D-5498CDEB23EF}" name="Test case 4" dataDxfId="96"/>
+    <tableColumn id="1" xr3:uid="{EA26578D-A990-4EA9-9A5D-5498CDEB23EF}" name="Test case 4" dataDxfId="114"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5811,10 +6430,10 @@
 </file>
 
 <file path=xl/tables/table40.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="50" xr:uid="{A1E6532E-E7F9-463F-AB12-75B62A6FFDB2}" name="Table614161841" displayName="Table614161841" ref="Q18:Q24" totalsRowShown="0" dataDxfId="95">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="50" xr:uid="{A1E6532E-E7F9-463F-AB12-75B62A6FFDB2}" name="Table614161841" displayName="Table614161841" ref="Q18:Q24" totalsRowShown="0" dataDxfId="113">
   <autoFilter ref="Q18:Q24" xr:uid="{A1E6532E-E7F9-463F-AB12-75B62A6FFDB2}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{62F2CC4D-8DD1-42DC-BE20-4D82AC53CCBB}" name="Test case 4" dataDxfId="94"/>
+    <tableColumn id="1" xr3:uid="{62F2CC4D-8DD1-42DC-BE20-4D82AC53CCBB}" name="Test case 4" dataDxfId="112"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5831,10 +6450,10 @@
 </file>
 
 <file path=xl/tables/table42.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="52" xr:uid="{1DF3B79D-BF1B-4769-AF92-820E9EC9A22E}" name="Table614161843" displayName="Table614161843" ref="Q26:Q32" totalsRowShown="0" dataDxfId="93">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="52" xr:uid="{1DF3B79D-BF1B-4769-AF92-820E9EC9A22E}" name="Table614161843" displayName="Table614161843" ref="Q26:Q32" totalsRowShown="0" dataDxfId="111">
   <autoFilter ref="Q26:Q32" xr:uid="{1DF3B79D-BF1B-4769-AF92-820E9EC9A22E}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{99055922-8FC6-4CBF-A5E8-2D242ACB7E2E}" name="Test case 4" dataDxfId="92"/>
+    <tableColumn id="1" xr3:uid="{99055922-8FC6-4CBF-A5E8-2D242ACB7E2E}" name="Test case 4" dataDxfId="110"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5851,10 +6470,10 @@
 </file>
 
 <file path=xl/tables/table44.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="54" xr:uid="{0858262B-88CB-42C1-A4D1-2D3C25384308}" name="Table614161845" displayName="Table614161845" ref="Q34:Q40" totalsRowShown="0" dataDxfId="91">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="54" xr:uid="{0858262B-88CB-42C1-A4D1-2D3C25384308}" name="Table614161845" displayName="Table614161845" ref="Q34:Q40" totalsRowShown="0" dataDxfId="109">
   <autoFilter ref="Q34:Q40" xr:uid="{0858262B-88CB-42C1-A4D1-2D3C25384308}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{F24CD206-65CA-4D44-ABC5-24D53E385DA0}" name="Test case 4" dataDxfId="90"/>
+    <tableColumn id="1" xr3:uid="{F24CD206-65CA-4D44-ABC5-24D53E385DA0}" name="Test case 4" dataDxfId="108"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5874,10 +6493,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="56" xr:uid="{8831F409-C230-4BD6-A3F6-305E39E147F2}" name="Table46" displayName="Table46" ref="V3:Y8" totalsRowShown="0">
   <autoFilter ref="V3:Y8" xr:uid="{8831F409-C230-4BD6-A3F6-305E39E147F2}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{EF0C86F3-D1BF-470E-9983-F2566B3C059B}" name="Num of Trees" dataDxfId="89"/>
+    <tableColumn id="1" xr3:uid="{EF0C86F3-D1BF-470E-9983-F2566B3C059B}" name="Num of Trees" dataDxfId="107"/>
     <tableColumn id="2" xr3:uid="{894F29E9-66C3-4DED-B821-ADEF4CC3256D}" name="Accuracy (%)"/>
     <tableColumn id="3" xr3:uid="{F5AF8A33-381A-4BA6-80A7-E805456FF17F}" name="Time taken (t) / s"/>
-    <tableColumn id="5" xr3:uid="{13C33019-312A-4AB7-8FCA-C67285781E3A}" name="Performance (1/t)" dataDxfId="88"/>
+    <tableColumn id="5" xr3:uid="{13C33019-312A-4AB7-8FCA-C67285781E3A}" name="Performance (1/t)" dataDxfId="106"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5887,10 +6506,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="57" xr:uid="{312BE8E0-A1AA-48FA-AB24-BA564DE3C8ED}" name="Table4658" displayName="Table4658" ref="V11:Y16" totalsRowShown="0">
   <autoFilter ref="V11:Y16" xr:uid="{312BE8E0-A1AA-48FA-AB24-BA564DE3C8ED}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{1E678731-A703-4D09-8C80-CD978ADC0E9D}" name="Num of Trees" dataDxfId="87"/>
+    <tableColumn id="1" xr3:uid="{1E678731-A703-4D09-8C80-CD978ADC0E9D}" name="Num of Trees" dataDxfId="105"/>
     <tableColumn id="2" xr3:uid="{339D92B4-F00C-4718-96E7-6F721BB2D010}" name="Accuracy (%)"/>
     <tableColumn id="3" xr3:uid="{9030AFB5-DC92-427A-80B2-D0760000BE59}" name="Time taken (t) / s"/>
-    <tableColumn id="5" xr3:uid="{1AD86E09-7658-4875-A0A6-69077B079556}" name="Performance (1/t)" dataDxfId="86"/>
+    <tableColumn id="5" xr3:uid="{1AD86E09-7658-4875-A0A6-69077B079556}" name="Performance (1/t)" dataDxfId="104"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5900,10 +6519,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="58" xr:uid="{517DB546-A1E6-430F-900F-CC75C5749164}" name="Table465859" displayName="Table465859" ref="V19:Y24" totalsRowShown="0">
   <autoFilter ref="V19:Y24" xr:uid="{517DB546-A1E6-430F-900F-CC75C5749164}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{DB945E36-427E-4801-AB6A-2C007584972C}" name="Num of Trees" dataDxfId="85"/>
-    <tableColumn id="2" xr3:uid="{8979CD11-B645-4437-956E-F2832987C36A}" name="Accuracy (%)" dataDxfId="84"/>
+    <tableColumn id="1" xr3:uid="{DB945E36-427E-4801-AB6A-2C007584972C}" name="Num of Trees" dataDxfId="103"/>
+    <tableColumn id="2" xr3:uid="{8979CD11-B645-4437-956E-F2832987C36A}" name="Accuracy (%)" dataDxfId="102"/>
     <tableColumn id="3" xr3:uid="{0ED2775B-431B-4718-818D-3F838EFCC388}" name="Time taken (t) / s"/>
-    <tableColumn id="5" xr3:uid="{9B47FF01-28EE-4239-8303-D51853E5E53F}" name="Performance (1/t)" dataDxfId="83"/>
+    <tableColumn id="5" xr3:uid="{9B47FF01-28EE-4239-8303-D51853E5E53F}" name="Performance (1/t)" dataDxfId="101"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5913,10 +6532,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{24818C57-3003-4ACB-BE4C-9B8E476F2C6F}" name="Table46585927" displayName="Table46585927" ref="V27:Y32" totalsRowShown="0">
   <autoFilter ref="V27:Y32" xr:uid="{24818C57-3003-4ACB-BE4C-9B8E476F2C6F}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{D4C1E20E-FF3B-4A51-B744-6295994F0870}" name="Num of Trees" dataDxfId="82"/>
+    <tableColumn id="1" xr3:uid="{D4C1E20E-FF3B-4A51-B744-6295994F0870}" name="Num of Trees" dataDxfId="100"/>
     <tableColumn id="2" xr3:uid="{59F07C21-015B-48F7-A874-C41C71EA4BE1}" name="Accuracy (%)"/>
     <tableColumn id="3" xr3:uid="{9661D1C0-60F4-4A46-9575-D5CCB98AC717}" name="Time taken (t) / s"/>
-    <tableColumn id="5" xr3:uid="{9573B299-328C-474E-A194-223EB7403867}" name="Performance (1/t)" dataDxfId="81"/>
+    <tableColumn id="5" xr3:uid="{9573B299-328C-474E-A194-223EB7403867}" name="Performance (1/t)" dataDxfId="99"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5933,10 +6552,10 @@
 </file>
 
 <file path=xl/tables/table50.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="27" xr:uid="{D64362BC-047A-43EC-9A44-D4237434B716}" name="Table62265" displayName="Table62265" ref="B2:B8" totalsRowShown="0" dataDxfId="80">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="27" xr:uid="{D64362BC-047A-43EC-9A44-D4237434B716}" name="Table62265" displayName="Table62265" ref="B2:B8" totalsRowShown="0" dataDxfId="98">
   <autoFilter ref="B2:B8" xr:uid="{D64362BC-047A-43EC-9A44-D4237434B716}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{123C3260-69F7-4AFD-97EA-602CB23358D3}" name="Test case 1.0" dataDxfId="79"/>
+    <tableColumn id="1" xr3:uid="{123C3260-69F7-4AFD-97EA-602CB23358D3}" name="Test case 1.0" dataDxfId="97"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5953,10 +6572,10 @@
 </file>
 
 <file path=xl/tables/table52.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="29" xr:uid="{2E62DF93-8030-47F7-81BB-5A56F89C919C}" name="Table6226567" displayName="Table6226567" ref="B10:B16" totalsRowShown="0" dataDxfId="78">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="29" xr:uid="{2E62DF93-8030-47F7-81BB-5A56F89C919C}" name="Table6226567" displayName="Table6226567" ref="B10:B16" totalsRowShown="0" dataDxfId="96">
   <autoFilter ref="B10:B16" xr:uid="{2E62DF93-8030-47F7-81BB-5A56F89C919C}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{A75BC07C-8537-4DDB-B30D-3886B55A56F4}" name="Test case 1.0" dataDxfId="77"/>
+    <tableColumn id="1" xr3:uid="{A75BC07C-8537-4DDB-B30D-3886B55A56F4}" name="Test case 1.0" dataDxfId="95"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5973,10 +6592,10 @@
 </file>
 
 <file path=xl/tables/table54.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="31" xr:uid="{6ABBF735-6A67-43CA-9700-86E361BE617E}" name="Table6226569" displayName="Table6226569" ref="B18:B24" totalsRowShown="0" dataDxfId="76">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="31" xr:uid="{6ABBF735-6A67-43CA-9700-86E361BE617E}" name="Table6226569" displayName="Table6226569" ref="B18:B24" totalsRowShown="0" dataDxfId="94">
   <autoFilter ref="B18:B24" xr:uid="{6ABBF735-6A67-43CA-9700-86E361BE617E}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{DA7968BA-6FD1-4C84-98F4-243204FA549E}" name="Test case 1.0" dataDxfId="75"/>
+    <tableColumn id="1" xr3:uid="{DA7968BA-6FD1-4C84-98F4-243204FA549E}" name="Test case 1.0" dataDxfId="93"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5993,10 +6612,10 @@
 </file>
 
 <file path=xl/tables/table56.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="33" xr:uid="{AE249DE3-A5D1-47D5-9E41-29DA2525FBD5}" name="Table6226571" displayName="Table6226571" ref="B26:B32" totalsRowShown="0" dataDxfId="74">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="33" xr:uid="{AE249DE3-A5D1-47D5-9E41-29DA2525FBD5}" name="Table6226571" displayName="Table6226571" ref="B26:B32" totalsRowShown="0" dataDxfId="92">
   <autoFilter ref="B26:B32" xr:uid="{AE249DE3-A5D1-47D5-9E41-29DA2525FBD5}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{C36085D3-57FF-4BA0-A217-50DF8094946E}" name="Test case 1.0" dataDxfId="73"/>
+    <tableColumn id="1" xr3:uid="{C36085D3-57FF-4BA0-A217-50DF8094946E}" name="Test case 1.0" dataDxfId="91"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6013,10 +6632,10 @@
 </file>
 
 <file path=xl/tables/table58.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="35" xr:uid="{8D786210-D16E-44EC-A5FC-B92AE2D1EB1C}" name="Table6226573" displayName="Table6226573" ref="B34:B40" totalsRowShown="0" dataDxfId="72">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="35" xr:uid="{8D786210-D16E-44EC-A5FC-B92AE2D1EB1C}" name="Table6226573" displayName="Table6226573" ref="B34:B40" totalsRowShown="0" dataDxfId="90">
   <autoFilter ref="B34:B40" xr:uid="{8D786210-D16E-44EC-A5FC-B92AE2D1EB1C}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{444CB8B2-FF7D-4C7F-AF91-CE356302558A}" name="Test case 1.0" dataDxfId="71"/>
+    <tableColumn id="1" xr3:uid="{444CB8B2-FF7D-4C7F-AF91-CE356302558A}" name="Test case 1.0" dataDxfId="89"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6033,20 +6652,20 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{4E98FA49-9DB8-4DDD-AD32-E514DB49B9C4}" name="Table6" displayName="Table6" ref="B10:B16" totalsRowShown="0" dataDxfId="129">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{4E98FA49-9DB8-4DDD-AD32-E514DB49B9C4}" name="Table6" displayName="Table6" ref="B10:B16" totalsRowShown="0" dataDxfId="147">
   <autoFilter ref="B10:B16" xr:uid="{4E98FA49-9DB8-4DDD-AD32-E514DB49B9C4}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{243A6057-BCFB-4C75-8BE6-2AD41CB2DBDC}" name="Test case 1.1" dataDxfId="128"/>
+    <tableColumn id="1" xr3:uid="{243A6057-BCFB-4C75-8BE6-2AD41CB2DBDC}" name="Test case 1.1" dataDxfId="146"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table60.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="60" xr:uid="{9C644C1A-1A63-4D23-B8DA-A973304493CC}" name="Table6226575" displayName="Table6226575" ref="B42:B48" totalsRowShown="0" dataDxfId="70">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="60" xr:uid="{9C644C1A-1A63-4D23-B8DA-A973304493CC}" name="Table6226575" displayName="Table6226575" ref="B42:B48" totalsRowShown="0" dataDxfId="88">
   <autoFilter ref="B42:B48" xr:uid="{9C644C1A-1A63-4D23-B8DA-A973304493CC}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{CE323FB7-B9DC-44E7-A42A-E4D92F4184F2}" name="Test case 1.0" dataDxfId="69"/>
+    <tableColumn id="1" xr3:uid="{CE323FB7-B9DC-44E7-A42A-E4D92F4184F2}" name="Test case 1.0" dataDxfId="87"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6073,10 +6692,10 @@
 </file>
 
 <file path=xl/tables/table63.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="63" xr:uid="{26E8E97E-FD63-4981-B7F9-22A8A88A30E8}" name="Table6143052" displayName="Table6143052" ref="G2:G8" totalsRowShown="0" dataDxfId="68">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="63" xr:uid="{26E8E97E-FD63-4981-B7F9-22A8A88A30E8}" name="Table6143052" displayName="Table6143052" ref="G2:G8" totalsRowShown="0" dataDxfId="86">
   <autoFilter ref="G2:G8" xr:uid="{26E8E97E-FD63-4981-B7F9-22A8A88A30E8}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{7A242E72-4CCA-486B-9C2C-B2A3553B6504}" name="Test case 2.0" dataDxfId="67"/>
+    <tableColumn id="1" xr3:uid="{7A242E72-4CCA-486B-9C2C-B2A3553B6504}" name="Test case 2.0" dataDxfId="85"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6093,10 +6712,10 @@
 </file>
 
 <file path=xl/tables/table65.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="65" xr:uid="{6A23E860-3DA8-4F20-AFAE-59EC1B83C630}" name="Table614305254" displayName="Table614305254" ref="G10:G16" totalsRowShown="0" dataDxfId="66">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="65" xr:uid="{6A23E860-3DA8-4F20-AFAE-59EC1B83C630}" name="Table614305254" displayName="Table614305254" ref="G10:G16" totalsRowShown="0" dataDxfId="84">
   <autoFilter ref="G10:G16" xr:uid="{6A23E860-3DA8-4F20-AFAE-59EC1B83C630}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{9208E1C2-E3C4-4E1D-BADA-B80EFDFBE8F1}" name="Test case 2.0" dataDxfId="65"/>
+    <tableColumn id="1" xr3:uid="{9208E1C2-E3C4-4E1D-BADA-B80EFDFBE8F1}" name="Test case 2.0" dataDxfId="83"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6113,10 +6732,10 @@
 </file>
 
 <file path=xl/tables/table67.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="67" xr:uid="{5465D290-D620-4A15-A2F8-52B3A46FFB29}" name="Table614305256" displayName="Table614305256" ref="G18:G24" totalsRowShown="0" dataDxfId="64">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="67" xr:uid="{5465D290-D620-4A15-A2F8-52B3A46FFB29}" name="Table614305256" displayName="Table614305256" ref="G18:G24" totalsRowShown="0" dataDxfId="82">
   <autoFilter ref="G18:G24" xr:uid="{5465D290-D620-4A15-A2F8-52B3A46FFB29}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{218687D0-4142-4F8D-8DB4-85D681EF8A97}" name="Test case 2.0" dataDxfId="63"/>
+    <tableColumn id="1" xr3:uid="{218687D0-4142-4F8D-8DB4-85D681EF8A97}" name="Test case 2.0" dataDxfId="81"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6133,10 +6752,10 @@
 </file>
 
 <file path=xl/tables/table69.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="69" xr:uid="{0EAAF75D-2BD3-487F-B377-78E8F46EE047}" name="Table614305258" displayName="Table614305258" ref="G26:G32" totalsRowShown="0" dataDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="69" xr:uid="{0EAAF75D-2BD3-487F-B377-78E8F46EE047}" name="Table614305258" displayName="Table614305258" ref="G26:G32" totalsRowShown="0" dataDxfId="80">
   <autoFilter ref="G26:G32" xr:uid="{0EAAF75D-2BD3-487F-B377-78E8F46EE047}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{47220119-16BF-471A-8532-966A2CBCB501}" name="Test case 2.0" dataDxfId="61"/>
+    <tableColumn id="1" xr3:uid="{47220119-16BF-471A-8532-966A2CBCB501}" name="Test case 2.0" dataDxfId="79"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6163,10 +6782,10 @@
 </file>
 
 <file path=xl/tables/table71.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="71" xr:uid="{850DCFE0-17CE-4D6D-8E50-F0CD3064CCD2}" name="Table614305260" displayName="Table614305260" ref="G34:G40" totalsRowShown="0" dataDxfId="60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="71" xr:uid="{850DCFE0-17CE-4D6D-8E50-F0CD3064CCD2}" name="Table614305260" displayName="Table614305260" ref="G34:G40" totalsRowShown="0" dataDxfId="78">
   <autoFilter ref="G34:G40" xr:uid="{850DCFE0-17CE-4D6D-8E50-F0CD3064CCD2}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{A50AD645-C3A3-4DC5-9D95-6C81764D08CD}" name="Test case 2.0" dataDxfId="59"/>
+    <tableColumn id="1" xr3:uid="{A50AD645-C3A3-4DC5-9D95-6C81764D08CD}" name="Test case 2.0" dataDxfId="77"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6183,20 +6802,20 @@
 </file>
 
 <file path=xl/tables/table73.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="73" xr:uid="{F01AE6E8-80F4-47C5-9EBB-093F892E91AC}" name="Table614305262" displayName="Table614305262" ref="G42:G48" totalsRowShown="0" dataDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="73" xr:uid="{F01AE6E8-80F4-47C5-9EBB-093F892E91AC}" name="Table614305262" displayName="Table614305262" ref="G42:G48" totalsRowShown="0" dataDxfId="76">
   <autoFilter ref="G42:G48" xr:uid="{F01AE6E8-80F4-47C5-9EBB-093F892E91AC}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{25F75ABF-75AE-4C4A-8475-EFABB3E35BEB}" name="Test case 2.0" dataDxfId="57"/>
+    <tableColumn id="1" xr3:uid="{25F75ABF-75AE-4C4A-8475-EFABB3E35BEB}" name="Test case 2.0" dataDxfId="75"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table74.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="74" xr:uid="{B68821F9-DDB9-4D95-B1B0-FA210E7BE89D}" name="Table6141675" displayName="Table6141675" ref="L2:L8" totalsRowShown="0" dataDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="74" xr:uid="{B68821F9-DDB9-4D95-B1B0-FA210E7BE89D}" name="Table6141675" displayName="Table6141675" ref="L2:L8" totalsRowShown="0" dataDxfId="74">
   <autoFilter ref="L2:L8" xr:uid="{B68821F9-DDB9-4D95-B1B0-FA210E7BE89D}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{2F969AE0-9DE6-485C-80D0-40EEB96177CF}" name="Test case 3.0" dataDxfId="55"/>
+    <tableColumn id="1" xr3:uid="{2F969AE0-9DE6-485C-80D0-40EEB96177CF}" name="Test case 3.0" dataDxfId="73"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6213,10 +6832,10 @@
 </file>
 
 <file path=xl/tables/table76.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="76" xr:uid="{F72EBC0E-55E3-44C5-9A52-7D09BC99FF4C}" name="Table614167577" displayName="Table614167577" ref="L10:L16" totalsRowShown="0" dataDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="76" xr:uid="{F72EBC0E-55E3-44C5-9A52-7D09BC99FF4C}" name="Table614167577" displayName="Table614167577" ref="L10:L16" totalsRowShown="0" dataDxfId="72">
   <autoFilter ref="L10:L16" xr:uid="{F72EBC0E-55E3-44C5-9A52-7D09BC99FF4C}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{30466062-40EE-4F8A-B39D-792FEA647E26}" name="Test case 3.0" dataDxfId="53"/>
+    <tableColumn id="1" xr3:uid="{30466062-40EE-4F8A-B39D-792FEA647E26}" name="Test case 3.0" dataDxfId="71"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6233,10 +6852,10 @@
 </file>
 
 <file path=xl/tables/table78.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="78" xr:uid="{3C14E2D7-4900-4F09-9366-C56F123F20E6}" name="Table614167579" displayName="Table614167579" ref="L18:L24" totalsRowShown="0" dataDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="78" xr:uid="{3C14E2D7-4900-4F09-9366-C56F123F20E6}" name="Table614167579" displayName="Table614167579" ref="L18:L24" totalsRowShown="0" dataDxfId="70">
   <autoFilter ref="L18:L24" xr:uid="{3C14E2D7-4900-4F09-9366-C56F123F20E6}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{BDA91CE6-D252-4E08-8227-F3252E4E0496}" name="Test case 3.0" dataDxfId="51"/>
+    <tableColumn id="1" xr3:uid="{BDA91CE6-D252-4E08-8227-F3252E4E0496}" name="Test case 3.0" dataDxfId="69"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6253,20 +6872,20 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{BE0A49AF-BE92-4702-8847-FC0E77169CAA}" name="Table622" displayName="Table622" ref="B2:B8" totalsRowShown="0" dataDxfId="127">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{BE0A49AF-BE92-4702-8847-FC0E77169CAA}" name="Table622" displayName="Table622" ref="B2:B8" totalsRowShown="0" dataDxfId="145">
   <autoFilter ref="B2:B8" xr:uid="{BE0A49AF-BE92-4702-8847-FC0E77169CAA}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{C4E7446A-9555-4E95-B603-150A9EBE6ABA}" name="Test case 1.0" dataDxfId="126"/>
+    <tableColumn id="1" xr3:uid="{C4E7446A-9555-4E95-B603-150A9EBE6ABA}" name="Test case 1.0" dataDxfId="144"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table80.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="80" xr:uid="{5B02E13E-1B0A-47EA-A534-CFA67829C450}" name="Table614167581" displayName="Table614167581" ref="L26:L32" totalsRowShown="0" dataDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="80" xr:uid="{5B02E13E-1B0A-47EA-A534-CFA67829C450}" name="Table614167581" displayName="Table614167581" ref="L26:L32" totalsRowShown="0" dataDxfId="68">
   <autoFilter ref="L26:L32" xr:uid="{5B02E13E-1B0A-47EA-A534-CFA67829C450}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{59862783-540E-4E51-BE80-B28EB585D709}" name="Test case 3.0" dataDxfId="49"/>
+    <tableColumn id="1" xr3:uid="{59862783-540E-4E51-BE80-B28EB585D709}" name="Test case 3.0" dataDxfId="67"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6283,10 +6902,10 @@
 </file>
 
 <file path=xl/tables/table82.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="82" xr:uid="{45207D75-3E85-469B-BA01-A38D85540773}" name="Table614167583" displayName="Table614167583" ref="L34:L40" totalsRowShown="0" dataDxfId="48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="82" xr:uid="{45207D75-3E85-469B-BA01-A38D85540773}" name="Table614167583" displayName="Table614167583" ref="L34:L40" totalsRowShown="0" dataDxfId="66">
   <autoFilter ref="L34:L40" xr:uid="{45207D75-3E85-469B-BA01-A38D85540773}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{0159D84D-3406-4095-BEDA-98C381B53FC7}" name="Test case 3.0" dataDxfId="47"/>
+    <tableColumn id="1" xr3:uid="{0159D84D-3406-4095-BEDA-98C381B53FC7}" name="Test case 3.0" dataDxfId="65"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6303,10 +6922,10 @@
 </file>
 
 <file path=xl/tables/table84.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="84" xr:uid="{0516D6A6-D6E8-4191-9778-B480A05DC44F}" name="Table614167585" displayName="Table614167585" ref="L42:L48" totalsRowShown="0" dataDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="84" xr:uid="{0516D6A6-D6E8-4191-9778-B480A05DC44F}" name="Table614167585" displayName="Table614167585" ref="L42:L48" totalsRowShown="0" dataDxfId="64">
   <autoFilter ref="L42:L48" xr:uid="{0516D6A6-D6E8-4191-9778-B480A05DC44F}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{2CA0230C-69C8-40D6-BFAD-CA5E926D027A}" name="Test case 3.0" dataDxfId="45"/>
+    <tableColumn id="1" xr3:uid="{2CA0230C-69C8-40D6-BFAD-CA5E926D027A}" name="Test case 3.0" dataDxfId="63"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6323,10 +6942,10 @@
 </file>
 
 <file path=xl/tables/table86.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="86" xr:uid="{E4AADACC-19A1-4C41-A0C9-B65507992DC2}" name="Table61416184387" displayName="Table61416184387" ref="Q2:Q8" totalsRowShown="0" dataDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="86" xr:uid="{E4AADACC-19A1-4C41-A0C9-B65507992DC2}" name="Table61416184387" displayName="Table61416184387" ref="Q2:Q8" totalsRowShown="0" dataDxfId="62">
   <autoFilter ref="Q2:Q8" xr:uid="{E4AADACC-19A1-4C41-A0C9-B65507992DC2}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{51878B36-D34B-46A5-BC1D-13D05933DD3D}" name="Test case 4" dataDxfId="43"/>
+    <tableColumn id="1" xr3:uid="{51878B36-D34B-46A5-BC1D-13D05933DD3D}" name="Test case 4" dataDxfId="61"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6343,10 +6962,10 @@
 </file>
 
 <file path=xl/tables/table88.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="88" xr:uid="{0F37C559-4DC8-4AA5-B444-8B6A3A1B1D5C}" name="Table6141618438789" displayName="Table6141618438789" ref="Q10:Q16" totalsRowShown="0" dataDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="88" xr:uid="{0F37C559-4DC8-4AA5-B444-8B6A3A1B1D5C}" name="Table6141618438789" displayName="Table6141618438789" ref="Q10:Q16" totalsRowShown="0" dataDxfId="60">
   <autoFilter ref="Q10:Q16" xr:uid="{0F37C559-4DC8-4AA5-B444-8B6A3A1B1D5C}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{7EB25CDF-A9A4-4AC6-8F83-1CD7D8D2156B}" name="Test case 4" dataDxfId="41"/>
+    <tableColumn id="1" xr3:uid="{7EB25CDF-A9A4-4AC6-8F83-1CD7D8D2156B}" name="Test case 4" dataDxfId="59"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6373,10 +6992,10 @@
 </file>
 
 <file path=xl/tables/table90.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="90" xr:uid="{34AB535A-5E67-49D2-AA09-D0684DFD05C7}" name="Table6141618438791" displayName="Table6141618438791" ref="Q18:Q24" totalsRowShown="0" dataDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="90" xr:uid="{34AB535A-5E67-49D2-AA09-D0684DFD05C7}" name="Table6141618438791" displayName="Table6141618438791" ref="Q18:Q24" totalsRowShown="0" dataDxfId="58">
   <autoFilter ref="Q18:Q24" xr:uid="{34AB535A-5E67-49D2-AA09-D0684DFD05C7}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{59F81A4D-53AD-4248-8CA3-D956A6E75CF5}" name="Test case 4" dataDxfId="39"/>
+    <tableColumn id="1" xr3:uid="{59F81A4D-53AD-4248-8CA3-D956A6E75CF5}" name="Test case 4" dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6393,10 +7012,10 @@
 </file>
 
 <file path=xl/tables/table92.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="92" xr:uid="{C6BD5C68-40B5-465C-8D86-85BADE8AFB80}" name="Table6141618438793" displayName="Table6141618438793" ref="Q26:Q32" totalsRowShown="0" dataDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="92" xr:uid="{C6BD5C68-40B5-465C-8D86-85BADE8AFB80}" name="Table6141618438793" displayName="Table6141618438793" ref="Q26:Q32" totalsRowShown="0" dataDxfId="56">
   <autoFilter ref="Q26:Q32" xr:uid="{C6BD5C68-40B5-465C-8D86-85BADE8AFB80}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{36A8F31A-3EC4-401D-99EB-0326CB3F5734}" name="Test case 4" dataDxfId="37"/>
+    <tableColumn id="1" xr3:uid="{36A8F31A-3EC4-401D-99EB-0326CB3F5734}" name="Test case 4" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6413,10 +7032,10 @@
 </file>
 
 <file path=xl/tables/table94.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="94" xr:uid="{C6BB2579-D18F-4CD2-BA2B-D640FDF4C2CE}" name="Table6141618438795" displayName="Table6141618438795" ref="Q34:Q40" totalsRowShown="0" dataDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="94" xr:uid="{C6BB2579-D18F-4CD2-BA2B-D640FDF4C2CE}" name="Table6141618438795" displayName="Table6141618438795" ref="Q34:Q40" totalsRowShown="0" dataDxfId="54">
   <autoFilter ref="Q34:Q40" xr:uid="{C6BB2579-D18F-4CD2-BA2B-D640FDF4C2CE}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{3EE10851-2B2B-4C3A-91CF-794EC920C47C}" name="Test case 4" dataDxfId="35"/>
+    <tableColumn id="1" xr3:uid="{3EE10851-2B2B-4C3A-91CF-794EC920C47C}" name="Test case 4" dataDxfId="53"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6433,10 +7052,10 @@
 </file>
 
 <file path=xl/tables/table96.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="96" xr:uid="{2C769679-EEFA-413B-842B-ACEC689CE1FF}" name="Table6141618438797" displayName="Table6141618438797" ref="Q42:Q48" totalsRowShown="0" dataDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="96" xr:uid="{2C769679-EEFA-413B-842B-ACEC689CE1FF}" name="Table6141618438797" displayName="Table6141618438797" ref="Q42:Q48" totalsRowShown="0" dataDxfId="52">
   <autoFilter ref="Q42:Q48" xr:uid="{2C769679-EEFA-413B-842B-ACEC689CE1FF}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{97225219-AECF-4BD4-9F88-52F1FECCF08A}" name="Test case 4" dataDxfId="33"/>
+    <tableColumn id="1" xr3:uid="{97225219-AECF-4BD4-9F88-52F1FECCF08A}" name="Test case 4" dataDxfId="51"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6456,10 +7075,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="98" xr:uid="{33A965EF-AE11-45FD-BB33-5DE8B592484E}" name="Table4699" displayName="Table4699" ref="V3:Y9" totalsRowShown="0">
   <autoFilter ref="V3:Y9" xr:uid="{33A965EF-AE11-45FD-BB33-5DE8B592484E}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{9836BA3F-BAE2-43DA-BCC9-ACE8977F2142}" name="Learning Rate" dataDxfId="32"/>
+    <tableColumn id="1" xr3:uid="{9836BA3F-BAE2-43DA-BCC9-ACE8977F2142}" name="Learning Rate" dataDxfId="50"/>
     <tableColumn id="2" xr3:uid="{759BD8BE-821C-4E96-9262-5B309F718400}" name="Accuracy (%)"/>
     <tableColumn id="3" xr3:uid="{0241B22C-D974-4588-9ACA-E54784E832F3}" name="Time taken (t) / s"/>
-    <tableColumn id="5" xr3:uid="{CB268E54-D66B-4912-A083-16A43DA0BE98}" name="Performance (1/t)" dataDxfId="31"/>
+    <tableColumn id="5" xr3:uid="{CB268E54-D66B-4912-A083-16A43DA0BE98}" name="Performance (1/t)" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6469,10 +7088,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="99" xr:uid="{2A7C3BFF-2D82-4709-95CA-239C04818150}" name="Table4658100" displayName="Table4658100" ref="V12:Y18" totalsRowShown="0">
   <autoFilter ref="V12:Y18" xr:uid="{2A7C3BFF-2D82-4709-95CA-239C04818150}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{7946E05E-550A-4BCD-991F-29B4A517BADD}" name="Learning Rate" dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{7946E05E-550A-4BCD-991F-29B4A517BADD}" name="Learning Rate" dataDxfId="48"/>
     <tableColumn id="2" xr3:uid="{F09AEF54-45C8-4E99-B57D-D93E94297FAB}" name="Accuracy (%)"/>
     <tableColumn id="3" xr3:uid="{C279033A-2B9B-4ED8-9EC2-D4DB9C91A394}" name="Time taken (t) / s"/>
-    <tableColumn id="5" xr3:uid="{F3637DE1-7768-4656-9AB0-DBFDD2AEEEF0}" name="Performance (1/t)" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{F3637DE1-7768-4656-9AB0-DBFDD2AEEEF0}" name="Performance (1/t)" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8690,8 +9309,8 @@
   </sheetPr>
   <dimension ref="B2:Y48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J18" sqref="G18:J24"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="Y2" sqref="V2:Y36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10733,10 +11352,10 @@
   <sheetPr codeName="Sheet4">
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="B2:J48"/>
+  <dimension ref="B2:T48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+    <sheetView tabSelected="1" topLeftCell="C10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q39" sqref="Q39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10745,9 +11364,15 @@
     <col min="5" max="5" width="11.140625" customWidth="1"/>
     <col min="7" max="7" width="16.85546875" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
+    <col min="12" max="12" width="25.85546875" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" customWidth="1"/>
+    <col min="17" max="17" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10">
+    <row r="2" spans="2:20" ht="20.25">
       <c r="B2" t="s">
         <v>12</v>
       </c>
@@ -10760,8 +11385,17 @@
       <c r="I2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="2:10">
+      <c r="L2" t="s">
+        <v>45</v>
+      </c>
+      <c r="N2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q2" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="2:20">
       <c r="B3" s="6" t="s">
         <v>14</v>
       </c>
@@ -10778,10 +11412,31 @@
         <v>15</v>
       </c>
       <c r="J3" s="7">
-        <v>161426934.268536</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10">
+        <v>1186850375.81757</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="N3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O3" s="7">
+        <v>850804799.31797898</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>72</v>
+      </c>
+      <c r="R3" t="s">
+        <v>49</v>
+      </c>
+      <c r="S3" t="s">
+        <v>50</v>
+      </c>
+      <c r="T3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="2:20">
       <c r="B4" s="6" t="s">
         <v>16</v>
       </c>
@@ -10798,10 +11453,31 @@
         <v>17</v>
       </c>
       <c r="J4" s="7">
-        <v>12705.3899691641</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10">
+        <v>34450.694852463697</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N4" t="s">
+        <v>17</v>
+      </c>
+      <c r="O4" s="7">
+        <v>29168.558403150098</v>
+      </c>
+      <c r="Q4" s="10">
+        <v>1</v>
+      </c>
+      <c r="R4">
+        <v>90</v>
+      </c>
+      <c r="S4">
+        <v>2</v>
+      </c>
+      <c r="T4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:20" ht="15.75" thickBot="1">
       <c r="B5" s="6" t="s">
         <v>55</v>
       </c>
@@ -10818,10 +11494,31 @@
         <v>19</v>
       </c>
       <c r="J5" s="7">
-        <v>8995.4083043003902</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10">
+        <v>26927.274866403801</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="N5" t="s">
+        <v>19</v>
+      </c>
+      <c r="O5" s="7">
+        <v>20828.636996257599</v>
+      </c>
+      <c r="Q5" s="10">
+        <v>2</v>
+      </c>
+      <c r="R5">
+        <v>98</v>
+      </c>
+      <c r="S5">
+        <v>2.4</v>
+      </c>
+      <c r="T5">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="6" spans="2:20" ht="15.75" thickBot="1">
       <c r="B6" s="6" t="s">
         <v>62</v>
       </c>
@@ -10832,16 +11529,37 @@
         <v>0.30000294905781399</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>20</v>
+        <v>62</v>
       </c>
       <c r="I6" t="s">
         <v>21</v>
       </c>
       <c r="J6" s="7">
-        <v>7.3872909280592203E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10">
+        <v>0.27342492005560298</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="N6" t="s">
+        <v>21</v>
+      </c>
+      <c r="O6" s="7">
+        <v>0.158130897739507</v>
+      </c>
+      <c r="Q6" s="17">
+        <v>3</v>
+      </c>
+      <c r="R6" s="18">
+        <v>99</v>
+      </c>
+      <c r="S6" s="18">
+        <v>2.1</v>
+      </c>
+      <c r="T6" s="19">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="7" spans="2:20">
       <c r="B7" s="6" t="s">
         <v>22</v>
       </c>
@@ -10858,10 +11576,31 @@
         <v>23</v>
       </c>
       <c r="J7" s="7">
-        <v>0.99069302827014405</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10">
+        <v>0.93157286331829303</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O7" s="7">
+        <v>0.95094736667856705</v>
+      </c>
+      <c r="Q7" s="10">
+        <v>4</v>
+      </c>
+      <c r="R7">
+        <v>99</v>
+      </c>
+      <c r="S7">
+        <v>2.7</v>
+      </c>
+      <c r="T7">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20">
       <c r="B8" s="6" t="s">
         <v>24</v>
       </c>
@@ -10878,10 +11617,45 @@
         <v>25</v>
       </c>
       <c r="J8" s="8">
-        <v>2.2999999999999998</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="N8" t="s">
+        <v>25</v>
+      </c>
+      <c r="O8" s="8">
+        <v>11.6</v>
+      </c>
+      <c r="Q8" s="10">
+        <v>5</v>
+      </c>
+      <c r="R8">
+        <v>99</v>
+      </c>
+      <c r="S8">
+        <v>2.9</v>
+      </c>
+      <c r="T8">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20">
+      <c r="Q9" s="10">
+        <v>6</v>
+      </c>
+      <c r="R9">
+        <v>99</v>
+      </c>
+      <c r="S9">
+        <v>2.9</v>
+      </c>
+      <c r="T9">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="10" spans="2:20">
       <c r="B10" t="s">
         <v>12</v>
       </c>
@@ -10894,8 +11668,14 @@
       <c r="I10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="2:10">
+      <c r="L10" t="s">
+        <v>45</v>
+      </c>
+      <c r="N10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="2:20" ht="20.25">
       <c r="B11" s="6" t="s">
         <v>14</v>
       </c>
@@ -10912,10 +11692,22 @@
         <v>15</v>
       </c>
       <c r="J11" s="7">
-        <v>161426934.268536</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10">
+        <v>281378440.22964102</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="N11" t="s">
+        <v>15</v>
+      </c>
+      <c r="O11" s="7">
+        <v>384076154.20521301</v>
+      </c>
+      <c r="Q11" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="2:20">
       <c r="B12" s="6" t="s">
         <v>16</v>
       </c>
@@ -10932,10 +11724,31 @@
         <v>17</v>
       </c>
       <c r="J12" s="7">
-        <v>12705.3899691641</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10">
+        <v>16774.338741948701</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N12" t="s">
+        <v>17</v>
+      </c>
+      <c r="O12" s="7">
+        <v>19597.860959941801</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>72</v>
+      </c>
+      <c r="R12" t="s">
+        <v>49</v>
+      </c>
+      <c r="S12" t="s">
+        <v>50</v>
+      </c>
+      <c r="T12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="2:20">
       <c r="B13" s="6" t="s">
         <v>55</v>
       </c>
@@ -10952,10 +11765,31 @@
         <v>19</v>
       </c>
       <c r="J13" s="7">
-        <v>8995.4083043003902</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10">
+        <v>12568.9312769801</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="N13" t="s">
+        <v>19</v>
+      </c>
+      <c r="O13" s="7">
+        <v>13482.463410738101</v>
+      </c>
+      <c r="Q13" s="10">
+        <v>1</v>
+      </c>
+      <c r="R13">
+        <v>93</v>
+      </c>
+      <c r="S13">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="T13">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="14" spans="2:20" ht="15.75" thickBot="1">
       <c r="B14" s="6" t="s">
         <v>63</v>
       </c>
@@ -10966,16 +11800,37 @@
         <v>0.13218779505995401</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="I14" t="s">
         <v>21</v>
       </c>
       <c r="J14" s="7">
-        <v>7.3872909280592203E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10">
+        <v>0.11291877378748399</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="N14" t="s">
+        <v>21</v>
+      </c>
+      <c r="O14" s="7">
+        <v>0.104016490336972</v>
+      </c>
+      <c r="Q14" s="10">
+        <v>2</v>
+      </c>
+      <c r="R14">
+        <v>98</v>
+      </c>
+      <c r="S14">
+        <v>2.4</v>
+      </c>
+      <c r="T14">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="15" spans="2:20" ht="15.75" thickBot="1">
       <c r="B15" s="6" t="s">
         <v>22</v>
       </c>
@@ -10992,10 +11847,31 @@
         <v>23</v>
       </c>
       <c r="J15" s="7">
-        <v>0.99069302827014405</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10">
+        <v>0.983777297137715</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N15" t="s">
+        <v>23</v>
+      </c>
+      <c r="O15" s="7">
+        <v>0.97785632289000102</v>
+      </c>
+      <c r="Q15" s="17">
+        <v>3</v>
+      </c>
+      <c r="R15" s="18">
+        <v>99</v>
+      </c>
+      <c r="S15" s="18">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="T15" s="19">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="16" spans="2:20">
       <c r="B16" s="6" t="s">
         <v>24</v>
       </c>
@@ -11012,10 +11888,45 @@
         <v>25</v>
       </c>
       <c r="J16" s="8">
+        <v>2.4</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="N16" t="s">
+        <v>25</v>
+      </c>
+      <c r="O16" s="8">
+        <v>22.5</v>
+      </c>
+      <c r="Q16" s="10">
+        <v>4</v>
+      </c>
+      <c r="R16">
+        <v>99</v>
+      </c>
+      <c r="S16">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="18" spans="2:10">
+      <c r="T16">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="17" spans="2:20">
+      <c r="Q17" s="10">
+        <v>5</v>
+      </c>
+      <c r="R17">
+        <v>99</v>
+      </c>
+      <c r="S17">
+        <v>2.4</v>
+      </c>
+      <c r="T17">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="18" spans="2:20">
       <c r="B18" t="s">
         <v>12</v>
       </c>
@@ -11028,8 +11939,26 @@
       <c r="I18" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="19" spans="2:10">
+      <c r="L18" t="s">
+        <v>45</v>
+      </c>
+      <c r="N18" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q18" s="10">
+        <v>6</v>
+      </c>
+      <c r="R18">
+        <v>99</v>
+      </c>
+      <c r="S18">
+        <v>2.4</v>
+      </c>
+      <c r="T18">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="19" spans="2:20">
       <c r="B19" s="6" t="s">
         <v>14</v>
       </c>
@@ -11048,8 +11977,17 @@
       <c r="J19" s="7">
         <v>161426934.268536</v>
       </c>
-    </row>
-    <row r="20" spans="2:10">
+      <c r="L19" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="N19" t="s">
+        <v>15</v>
+      </c>
+      <c r="O19" s="7">
+        <v>196398906.35940999</v>
+      </c>
+    </row>
+    <row r="20" spans="2:20" ht="20.25">
       <c r="B20" s="6" t="s">
         <v>16</v>
       </c>
@@ -11068,8 +12006,20 @@
       <c r="J20" s="7">
         <v>12705.3899691641</v>
       </c>
-    </row>
-    <row r="21" spans="2:10">
+      <c r="L20" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N20" t="s">
+        <v>17</v>
+      </c>
+      <c r="O20" s="7">
+        <v>14014.239414231801</v>
+      </c>
+      <c r="Q20" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="2:20">
       <c r="B21" s="6" t="s">
         <v>55</v>
       </c>
@@ -11088,8 +12038,29 @@
       <c r="J21" s="7">
         <v>8995.4083043003902</v>
       </c>
-    </row>
-    <row r="22" spans="2:10">
+      <c r="L21" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="N21" t="s">
+        <v>19</v>
+      </c>
+      <c r="O21" s="7">
+        <v>9418.2231885986002</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>72</v>
+      </c>
+      <c r="R21" t="s">
+        <v>49</v>
+      </c>
+      <c r="S21" t="s">
+        <v>50</v>
+      </c>
+      <c r="T21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="2:20">
       <c r="B22" s="6" t="s">
         <v>20</v>
       </c>
@@ -11108,8 +12079,29 @@
       <c r="J22" s="7">
         <v>7.3872909280592203E-2</v>
       </c>
-    </row>
-    <row r="23" spans="2:10">
+      <c r="L22" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N22" t="s">
+        <v>21</v>
+      </c>
+      <c r="O22" s="7">
+        <v>7.1039840098551299E-2</v>
+      </c>
+      <c r="Q22" s="10">
+        <v>1</v>
+      </c>
+      <c r="R22">
+        <v>95</v>
+      </c>
+      <c r="S22">
+        <v>11.6</v>
+      </c>
+      <c r="T22">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="23" spans="2:20" ht="15.75" thickBot="1">
       <c r="B23" s="6" t="s">
         <v>22</v>
       </c>
@@ -11128,8 +12120,29 @@
       <c r="J23" s="7">
         <v>0.99069302827014405</v>
       </c>
-    </row>
-    <row r="24" spans="2:10">
+      <c r="L23" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N23" t="s">
+        <v>23</v>
+      </c>
+      <c r="O23" s="7">
+        <v>0.98867674048606502</v>
+      </c>
+      <c r="Q23" s="10">
+        <v>2</v>
+      </c>
+      <c r="R23">
+        <v>98</v>
+      </c>
+      <c r="S23">
+        <v>22.5</v>
+      </c>
+      <c r="T23">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="24" spans="2:20" ht="15.75" thickBot="1">
       <c r="B24" s="6" t="s">
         <v>24</v>
       </c>
@@ -11148,8 +12161,43 @@
       <c r="J24" s="8">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="26" spans="2:10">
+      <c r="L24" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="N24" t="s">
+        <v>25</v>
+      </c>
+      <c r="O24" s="8">
+        <v>32.9</v>
+      </c>
+      <c r="Q24" s="17">
+        <v>3</v>
+      </c>
+      <c r="R24" s="18">
+        <v>99</v>
+      </c>
+      <c r="S24" s="18">
+        <v>32.9</v>
+      </c>
+      <c r="T24" s="19">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="25" spans="2:20">
+      <c r="Q25" s="10">
+        <v>4</v>
+      </c>
+      <c r="R25">
+        <v>99</v>
+      </c>
+      <c r="S25">
+        <v>40.299999999999997</v>
+      </c>
+      <c r="T25">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="26" spans="2:20">
       <c r="B26" t="s">
         <v>12</v>
       </c>
@@ -11162,8 +12210,26 @@
       <c r="I26" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="27" spans="2:10">
+      <c r="L26" t="s">
+        <v>45</v>
+      </c>
+      <c r="N26" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q26" s="10">
+        <v>5</v>
+      </c>
+      <c r="R26">
+        <v>99</v>
+      </c>
+      <c r="S26">
+        <v>58.1</v>
+      </c>
+      <c r="T26">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="27" spans="2:20">
       <c r="B27" s="6" t="s">
         <v>14</v>
       </c>
@@ -11180,10 +12246,31 @@
         <v>15</v>
       </c>
       <c r="J27" s="7">
-        <v>161426934.268536</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10">
+        <v>91013012.1284578</v>
+      </c>
+      <c r="L27" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="N27" t="s">
+        <v>15</v>
+      </c>
+      <c r="O27" s="7">
+        <v>116824187.352469</v>
+      </c>
+      <c r="Q27" s="10">
+        <v>6</v>
+      </c>
+      <c r="R27">
+        <v>99</v>
+      </c>
+      <c r="S27">
+        <v>76.5</v>
+      </c>
+      <c r="T27">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="28" spans="2:20">
       <c r="B28" s="6" t="s">
         <v>16</v>
       </c>
@@ -11200,10 +12287,19 @@
         <v>17</v>
       </c>
       <c r="J28" s="7">
-        <v>12705.3899691641</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10">
+        <v>9540.0740106383801</v>
+      </c>
+      <c r="L28" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N28" t="s">
+        <v>17</v>
+      </c>
+      <c r="O28" s="7">
+        <v>10808.523828556299</v>
+      </c>
+    </row>
+    <row r="29" spans="2:20">
       <c r="B29" s="6" t="s">
         <v>55</v>
       </c>
@@ -11220,10 +12316,19 @@
         <v>19</v>
       </c>
       <c r="J29" s="7">
-        <v>8995.4083043003902</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10">
+        <v>6169.7572421053801</v>
+      </c>
+      <c r="L29" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="N29" t="s">
+        <v>19</v>
+      </c>
+      <c r="O29" s="7">
+        <v>6900.8462021496998</v>
+      </c>
+    </row>
+    <row r="30" spans="2:20">
       <c r="B30" s="6" t="s">
         <v>64</v>
       </c>
@@ -11234,16 +12339,25 @@
         <v>5.4058913058424203E-2</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="I30" t="s">
         <v>21</v>
       </c>
       <c r="J30" s="7">
-        <v>7.3872909280592203E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10">
+        <v>5.0367204285042801E-2</v>
+      </c>
+      <c r="L30" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="N30" t="s">
+        <v>21</v>
+      </c>
+      <c r="O30" s="7">
+        <v>5.4239439311091903E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:20">
       <c r="B31" s="6" t="s">
         <v>22</v>
       </c>
@@ -11260,10 +12374,19 @@
         <v>23</v>
       </c>
       <c r="J31" s="7">
-        <v>0.99069302827014405</v>
-      </c>
-    </row>
-    <row r="32" spans="2:10">
+        <v>0.99475270013169204</v>
+      </c>
+      <c r="L31" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N31" t="s">
+        <v>23</v>
+      </c>
+      <c r="O31" s="7">
+        <v>0.99326457252019595</v>
+      </c>
+    </row>
+    <row r="32" spans="2:20">
       <c r="B32" s="6" t="s">
         <v>24</v>
       </c>
@@ -11282,8 +12405,17 @@
       <c r="J32" s="8">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="34" spans="2:10">
+      <c r="L32" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="N32" t="s">
+        <v>25</v>
+      </c>
+      <c r="O32" s="8">
+        <v>40.299999999999997</v>
+      </c>
+    </row>
+    <row r="34" spans="2:15">
       <c r="B34" t="s">
         <v>12</v>
       </c>
@@ -11296,8 +12428,14 @@
       <c r="I34" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="35" spans="2:10">
+      <c r="L34" t="s">
+        <v>45</v>
+      </c>
+      <c r="N34" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="2:15">
       <c r="B35" s="6" t="s">
         <v>14</v>
       </c>
@@ -11314,10 +12452,19 @@
         <v>15</v>
       </c>
       <c r="J35" s="7">
-        <v>161426934.268536</v>
-      </c>
-    </row>
-    <row r="36" spans="2:10">
+        <v>59401263.510237098</v>
+      </c>
+      <c r="L35" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="N35" t="s">
+        <v>15</v>
+      </c>
+      <c r="O35" s="7">
+        <v>83175083.400143102</v>
+      </c>
+    </row>
+    <row r="36" spans="2:15">
       <c r="B36" s="6" t="s">
         <v>16</v>
       </c>
@@ -11334,10 +12481,19 @@
         <v>17</v>
       </c>
       <c r="J36" s="7">
-        <v>12705.3899691641</v>
-      </c>
-    </row>
-    <row r="37" spans="2:10">
+        <v>7707.2215168786397</v>
+      </c>
+      <c r="L36" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N36" t="s">
+        <v>17</v>
+      </c>
+      <c r="O36" s="7">
+        <v>9120.0374670361507</v>
+      </c>
+    </row>
+    <row r="37" spans="2:15">
       <c r="B37" s="6" t="s">
         <v>55</v>
       </c>
@@ -11354,10 +12510,19 @@
         <v>19</v>
       </c>
       <c r="J37" s="7">
-        <v>8995.4083043003902</v>
-      </c>
-    </row>
-    <row r="38" spans="2:10">
+        <v>4718.73271513701</v>
+      </c>
+      <c r="L37" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="N37" t="s">
+        <v>19</v>
+      </c>
+      <c r="O37" s="7">
+        <v>5600.0924998201399</v>
+      </c>
+    </row>
+    <row r="38" spans="2:15">
       <c r="B38" s="6" t="s">
         <v>65</v>
       </c>
@@ -11368,16 +12533,25 @@
         <v>4.0027528307112599E-2</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>20</v>
+        <v>65</v>
       </c>
       <c r="I38" t="s">
         <v>21</v>
       </c>
       <c r="J38" s="7">
-        <v>7.3872909280592203E-2</v>
-      </c>
-    </row>
-    <row r="39" spans="2:10">
+        <v>4.0155301274366E-2</v>
+      </c>
+      <c r="L38" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="N38" t="s">
+        <v>21</v>
+      </c>
+      <c r="O38" s="7">
+        <v>4.3819210134194E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:15">
       <c r="B39" s="6" t="s">
         <v>22</v>
       </c>
@@ -11394,10 +12568,19 @@
         <v>23</v>
       </c>
       <c r="J39" s="7">
-        <v>0.99069302827014405</v>
-      </c>
-    </row>
-    <row r="40" spans="2:10">
+        <v>0.996575256274843</v>
+      </c>
+      <c r="L39" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N39" t="s">
+        <v>23</v>
+      </c>
+      <c r="O39" s="7">
+        <v>0.99520459114619697</v>
+      </c>
+    </row>
+    <row r="40" spans="2:15">
       <c r="B40" s="6" t="s">
         <v>24</v>
       </c>
@@ -11414,10 +12597,19 @@
         <v>25</v>
       </c>
       <c r="J40" s="8">
-        <v>2.2999999999999998</v>
-      </c>
-    </row>
-    <row r="42" spans="2:10">
+        <v>2.4</v>
+      </c>
+      <c r="L40" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="N40" t="s">
+        <v>25</v>
+      </c>
+      <c r="O40" s="8">
+        <v>58.7</v>
+      </c>
+    </row>
+    <row r="42" spans="2:15">
       <c r="B42" t="s">
         <v>12</v>
       </c>
@@ -11430,8 +12622,14 @@
       <c r="I42" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="43" spans="2:10">
+      <c r="L42" t="s">
+        <v>45</v>
+      </c>
+      <c r="N42" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="2:15">
       <c r="B43" s="6" t="s">
         <v>14</v>
       </c>
@@ -11448,10 +12646,19 @@
         <v>15</v>
       </c>
       <c r="J43" s="7">
-        <v>161426934.268536</v>
-      </c>
-    </row>
-    <row r="44" spans="2:10">
+        <v>49048470.290383898</v>
+      </c>
+      <c r="L43" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="N43" t="s">
+        <v>15</v>
+      </c>
+      <c r="O43" s="7">
+        <v>67716778.731985897</v>
+      </c>
+    </row>
+    <row r="44" spans="2:15">
       <c r="B44" s="6" t="s">
         <v>16</v>
       </c>
@@ -11468,10 +12675,19 @@
         <v>17</v>
       </c>
       <c r="J44" s="7">
-        <v>12705.3899691641</v>
-      </c>
-    </row>
-    <row r="45" spans="2:10">
+        <v>7003.4613078379998</v>
+      </c>
+      <c r="L44" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N44" t="s">
+        <v>17</v>
+      </c>
+      <c r="O44" s="7">
+        <v>8229.0205208144798</v>
+      </c>
+    </row>
+    <row r="45" spans="2:15">
       <c r="B45" s="6" t="s">
         <v>55</v>
       </c>
@@ -11488,10 +12704,19 @@
         <v>19</v>
       </c>
       <c r="J45" s="7">
-        <v>8995.4083043003902</v>
-      </c>
-    </row>
-    <row r="46" spans="2:10">
+        <v>3940.7650951732899</v>
+      </c>
+      <c r="L45" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="N45" t="s">
+        <v>19</v>
+      </c>
+      <c r="O45" s="7">
+        <v>4869.6959709796802</v>
+      </c>
+    </row>
+    <row r="46" spans="2:15">
       <c r="B46" s="6" t="s">
         <v>66</v>
       </c>
@@ -11502,16 +12727,25 @@
         <v>3.2400394510328702E-2</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="I46" t="s">
         <v>21</v>
       </c>
       <c r="J46" s="7">
-        <v>7.3872909280592203E-2</v>
-      </c>
-    </row>
-    <row r="47" spans="2:10">
+        <v>3.3506305336325801E-2</v>
+      </c>
+      <c r="L46" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="N46" t="s">
+        <v>21</v>
+      </c>
+      <c r="O46" s="7">
+        <v>3.8643773142845998E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="2:15">
       <c r="B47" s="6" t="s">
         <v>22</v>
       </c>
@@ -11528,10 +12762,19 @@
         <v>23</v>
       </c>
       <c r="J47" s="7">
-        <v>0.99069302827014405</v>
-      </c>
-    </row>
-    <row r="48" spans="2:10">
+        <v>0.99717214027229195</v>
+      </c>
+      <c r="L47" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N47" t="s">
+        <v>23</v>
+      </c>
+      <c r="O47" s="7">
+        <v>0.99609583030148396</v>
+      </c>
+    </row>
+    <row r="48" spans="2:15">
       <c r="B48" s="6" t="s">
         <v>24</v>
       </c>
@@ -11548,7 +12791,16 @@
         <v>25</v>
       </c>
       <c r="J48" s="8">
-        <v>2.2999999999999998</v>
+        <v>2.4</v>
+      </c>
+      <c r="L48" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="N48" t="s">
+        <v>25</v>
+      </c>
+      <c r="O48" s="8">
+        <v>76.5</v>
       </c>
     </row>
   </sheetData>
@@ -11564,16 +12816,16 @@
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[0]!CalculateAverage">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
-                    <xdr:col>18</xdr:col>
-                    <xdr:colOff>161925</xdr:colOff>
-                    <xdr:row>1</xdr:row>
-                    <xdr:rowOff>95250</xdr:rowOff>
+                    <xdr:col>20</xdr:col>
+                    <xdr:colOff>180975</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>20</xdr:col>
-                    <xdr:colOff>400050</xdr:colOff>
-                    <xdr:row>3</xdr:row>
-                    <xdr:rowOff>57150</xdr:rowOff>
+                    <xdr:col>22</xdr:col>
+                    <xdr:colOff>428625</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11586,16 +12838,16 @@
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[0]!ProcessData">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
-                    <xdr:col>18</xdr:col>
-                    <xdr:colOff>161925</xdr:colOff>
-                    <xdr:row>3</xdr:row>
-                    <xdr:rowOff>190500</xdr:rowOff>
+                    <xdr:col>20</xdr:col>
+                    <xdr:colOff>180975</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>152400</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>20</xdr:col>
-                    <xdr:colOff>400050</xdr:colOff>
-                    <xdr:row>5</xdr:row>
-                    <xdr:rowOff>152400</xdr:rowOff>
+                    <xdr:col>22</xdr:col>
+                    <xdr:colOff>428625</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>123825</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11608,15 +12860,15 @@
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[0]!CalculateReciprocals">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
-                    <xdr:col>18</xdr:col>
-                    <xdr:colOff>161925</xdr:colOff>
-                    <xdr:row>6</xdr:row>
-                    <xdr:rowOff>95250</xdr:rowOff>
+                    <xdr:col>20</xdr:col>
+                    <xdr:colOff>180975</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>76200</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>20</xdr:col>
-                    <xdr:colOff>400050</xdr:colOff>
-                    <xdr:row>8</xdr:row>
+                    <xdr:col>22</xdr:col>
+                    <xdr:colOff>428625</xdr:colOff>
+                    <xdr:row>9</xdr:row>
                     <xdr:rowOff>57150</xdr:rowOff>
                   </to>
                 </anchor>
@@ -11627,7 +12879,7 @@
       </controls>
     </mc:Choice>
   </mc:AlternateContent>
-  <tableParts count="24">
+  <tableParts count="39">
     <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
     <tablePart r:id="rId8"/>
@@ -11652,6 +12904,21 @@
     <tablePart r:id="rId27"/>
     <tablePart r:id="rId28"/>
     <tablePart r:id="rId29"/>
+    <tablePart r:id="rId30"/>
+    <tablePart r:id="rId31"/>
+    <tablePart r:id="rId32"/>
+    <tablePart r:id="rId33"/>
+    <tablePart r:id="rId34"/>
+    <tablePart r:id="rId35"/>
+    <tablePart r:id="rId36"/>
+    <tablePart r:id="rId37"/>
+    <tablePart r:id="rId38"/>
+    <tablePart r:id="rId39"/>
+    <tablePart r:id="rId40"/>
+    <tablePart r:id="rId41"/>
+    <tablePart r:id="rId42"/>
+    <tablePart r:id="rId43"/>
+    <tablePart r:id="rId44"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>